<commit_message>
extend the unit test to column C
</commit_message>
<xml_diff>
--- a/config/test.xlsx
+++ b/config/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aless\OneDrive\Desktop\SafeMove\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97216CA1-5BA1-47AD-B58A-560A2F0208B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B47D6F8B-F5F4-41AA-97DA-3B97876908EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13875" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-150" yWindow="83" windowWidth="23025" windowHeight="13665" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Angles" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="169">
   <si>
     <t>Tabella A</t>
   </si>
@@ -602,6 +602,24 @@
   </si>
   <si>
     <t>score.TableB</t>
+  </si>
+  <si>
+    <t>score.TableA.mean</t>
+  </si>
+  <si>
+    <t>score.TableB.mean</t>
+  </si>
+  <si>
+    <t>score.TableA.Tot</t>
+  </si>
+  <si>
+    <t>score.TableB.Tot</t>
+  </si>
+  <si>
+    <t>score.TableC</t>
+  </si>
+  <si>
+    <t>score.REBA</t>
   </si>
 </sst>
 </file>
@@ -1330,7 +1348,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="179">
+  <cellXfs count="180">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1628,6 +1646,75 @@
     <xf numFmtId="0" fontId="0" fillId="23" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="1" fontId="8" fillId="9" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1727,124 +1814,14 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="8" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCC66FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="8">
     <dxf>
       <font>
         <color theme="1"/>
@@ -27149,10 +27126,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87C26A6D-CC0D-478D-B939-E4C5166502FD}">
-  <dimension ref="A1:AE53"/>
+  <dimension ref="A1:AE54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="Q19" sqref="Q19"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="V19" sqref="V19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -27168,10 +27145,12 @@
     <col min="14" max="14" width="9.796875" style="2" customWidth="1"/>
     <col min="15" max="15" width="11.19921875" style="2" customWidth="1"/>
     <col min="16" max="17" width="14.9296875" style="2" customWidth="1"/>
-    <col min="19" max="20" width="8.86328125" style="2"/>
-    <col min="21" max="21" width="9.46484375" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="3.46484375" style="2" customWidth="1"/>
-    <col min="23" max="23" width="7.19921875" style="2" customWidth="1"/>
+    <col min="18" max="18" width="17.265625" customWidth="1"/>
+    <col min="19" max="19" width="17" style="2" customWidth="1"/>
+    <col min="20" max="20" width="15.33203125" style="2" customWidth="1"/>
+    <col min="21" max="21" width="14.73046875" style="2" customWidth="1"/>
+    <col min="22" max="22" width="14.3984375" style="2" customWidth="1"/>
+    <col min="23" max="23" width="15.33203125" style="2" customWidth="1"/>
     <col min="24" max="25" width="9.46484375" style="2" customWidth="1"/>
     <col min="26" max="26" width="8.86328125" style="2"/>
     <col min="27" max="27" width="2.86328125" style="2" customWidth="1"/>
@@ -27185,7 +27164,7 @@
     <col min="36" max="36" width="8.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>146</v>
       </c>
@@ -27237,206 +27216,181 @@
       <c r="Q1" s="5" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A2" s="106">
+      <c r="R1" s="179" t="s">
+        <v>163</v>
+      </c>
+      <c r="S1" s="179" t="s">
+        <v>164</v>
+      </c>
+      <c r="T1" s="179" t="s">
+        <v>165</v>
+      </c>
+      <c r="U1" s="179" t="s">
+        <v>166</v>
+      </c>
+      <c r="V1" s="179" t="s">
+        <v>167</v>
+      </c>
+      <c r="W1" s="179" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A2" s="2"/>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A3" s="106">
         <f>Angles!A3</f>
         <v>1</v>
       </c>
-      <c r="B2" s="2">
-        <f>IF(A2=0,0,IF(Scores!B3+Scores!C3+Scores!D3=1,1,IF(Scores!B3+Scores!C3+Scores!D3=2,2,IF(Scores!B3+Scores!C3+Scores!D3&gt;=3,3,0))))</f>
+      <c r="B3" s="2">
+        <f>IF(A3=0,0,IF(Scores!B3+Scores!C3+Scores!D3=1,1,IF(Scores!B3+Scores!C3+Scores!D3=2,2,IF(Scores!B3+Scores!C3+Scores!D3&gt;=3,3,0))))</f>
         <v>3</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C3" s="2">
         <f>Scores!E3+Scores!F3+Scores!G3</f>
         <v>5</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D3" s="2">
         <f>Scores!H3+Scores!I3</f>
         <v>5</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E3" s="2">
         <f>Scores!J3+Scores!K3</f>
         <v>3</v>
       </c>
-      <c r="F2" s="2">
-        <f>IF(D2&gt;E2,D2,E2)</f>
+      <c r="F3" s="2">
+        <f t="shared" ref="F3:F28" si="0">IF(D3&gt;E3,D3,E3)</f>
         <v>5</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G3" s="2">
         <f>Scores!L3</f>
         <v>2</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H3" s="2">
         <f>Scores!N3</f>
         <v>1</v>
       </c>
-      <c r="I2" s="2">
-        <f>IF(A2=0,0,IF(G2&gt;H2,G2,H2))</f>
-        <v>2</v>
-      </c>
-      <c r="J2" s="2">
+      <c r="I3" s="2">
+        <f t="shared" ref="I3:I28" si="1">IF(A3=0,0,IF(G3&gt;H3,G3,H3))</f>
+        <v>2</v>
+      </c>
+      <c r="J3" s="2">
         <f>Scores!P3+MAX(Scores!Q3,Scores!M3)</f>
         <v>2</v>
       </c>
-      <c r="K2" s="2">
+      <c r="K3" s="2">
         <f>Scores!R3+MAX(Scores!S3,Scores!O3)</f>
         <v>3</v>
       </c>
-      <c r="L2" s="2">
-        <f>IF(J2&gt;K2,J2,K2)</f>
+      <c r="L3" s="2">
+        <f t="shared" ref="L3:L28" si="2">IF(J3&gt;K3,J3,K3)</f>
         <v>3</v>
       </c>
-      <c r="M2" s="2">
+      <c r="M3" s="2">
         <f>Scores!T3+Scores!V3</f>
         <v>4</v>
       </c>
-      <c r="N2" s="2">
+      <c r="N3" s="2">
         <f>Scores!U3+Scores!V3</f>
         <v>2</v>
       </c>
-      <c r="O2" s="2">
-        <f>IF(M2&gt;N2,M2,N2)</f>
+      <c r="O3" s="2">
+        <f t="shared" ref="O3:O28" si="3">IF(M3&gt;N3,M3,N3)</f>
         <v>4</v>
       </c>
-      <c r="P2" s="5">
-        <f>IF(B2=0," ",IF(B2=Extra!$S$2,VLOOKUP(C2,Extra!$R$4:$AD$8,O2+1),IF(B2=Extra!$W$2,VLOOKUP(C2,Extra!$R$4:$AD$8,(O2+5)),IF(B2=Extra!$AA$2,VLOOKUP(C2,Extra!$R$4:$AD$8,(O2+9)),0))))</f>
+      <c r="P3" s="5">
+        <f>IF(B3=0," ",IF(B3=Extra!$S$2,VLOOKUP(C3,Extra!$R$4:$AD$8,O3+1),IF(B3=Extra!$W$2,VLOOKUP(C3,Extra!$R$4:$AD$8,(O3+5)),IF(B3=Extra!$AA$2,VLOOKUP(C3,Extra!$R$4:$AD$8,(O3+9)),0))))</f>
         <v>9</v>
       </c>
-      <c r="Q2" s="5">
-        <f>IF(I2=0," ",IF(I2=Extra!$S$10,VLOOKUP(F2,Extra!$R$12:$X$17,L2+1),IF(I2=Extra!$V$10,VLOOKUP(F2,Extra!$R$12:$X$17,(L2+4)),0)))</f>
+      <c r="Q3" s="5">
+        <f>IF(I3=0," ",IF(I3=Extra!$S$10,VLOOKUP(F3,Extra!$R$12:$X$17,L3+1),IF(I3=Extra!$V$10,VLOOKUP(F3,Extra!$R$12:$X$17,(L3+4)),0)))</f>
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A3" s="106">
+      <c r="R3">
+        <f>SUM(P3:P28)/26</f>
+        <v>4.7307692307692308</v>
+      </c>
+      <c r="S3">
+        <f>SUM(Q3:Q28)/26</f>
+        <v>2.5769230769230771</v>
+      </c>
+      <c r="T3">
+        <f>$R$3+3</f>
+        <v>7.7307692307692308</v>
+      </c>
+      <c r="U3">
+        <f>S3+2</f>
+        <v>4.5769230769230766</v>
+      </c>
+      <c r="V3">
+        <f>VLOOKUP(ROUND($T3,0),Extra!$S$21:$AE$32,ROUND($U3,0)+1)</f>
+        <v>10</v>
+      </c>
+      <c r="W3">
+        <f>V3+1</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A4" s="106">
         <f>Angles!A4</f>
         <v>2</v>
       </c>
-      <c r="B3" s="2">
-        <f>IF(A3=0,0,IF(Scores!B4+Scores!C4+Scores!D4=1,1,IF(Scores!B4+Scores!C4+Scores!D4=2,2,IF(Scores!B4+Scores!C4+Scores!D4&gt;=3,3,0))))</f>
+      <c r="B4" s="2">
+        <f>IF(A4=0,0,IF(Scores!B4+Scores!C4+Scores!D4=1,1,IF(Scores!B4+Scores!C4+Scores!D4=2,2,IF(Scores!B4+Scores!C4+Scores!D4&gt;=3,3,0))))</f>
         <v>3</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C4" s="2">
         <f>Scores!E4+Scores!F4+Scores!G4</f>
         <v>4</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D4" s="2">
         <f>Scores!H4+Scores!I4</f>
         <v>4</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E4" s="2">
         <f>Scores!J4+Scores!K4</f>
         <v>2</v>
       </c>
-      <c r="F3" s="2">
-        <f>IF(D3&gt;E3,D3,E3)</f>
+      <c r="F4" s="2">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G4" s="2">
         <f>Scores!L4</f>
         <v>2</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H4" s="2">
         <f>Scores!N4</f>
         <v>1</v>
       </c>
-      <c r="I3" s="2">
-        <f>IF(A3=0,0,IF(G3&gt;H3,G3,H3))</f>
-        <v>2</v>
-      </c>
-      <c r="J3" s="2">
+      <c r="I4" s="2">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="J4" s="2">
         <f>Scores!P4+MAX(Scores!Q4,Scores!M4)</f>
         <v>1</v>
       </c>
-      <c r="K3" s="2">
+      <c r="K4" s="2">
         <f>Scores!R4+MAX(Scores!S4,Scores!O4)</f>
         <v>2</v>
       </c>
-      <c r="L3" s="2">
-        <f>IF(J3&gt;K3,J3,K3)</f>
-        <v>2</v>
-      </c>
-      <c r="M3" s="2">
+      <c r="L4" s="2">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="M4" s="2">
         <f>Scores!T4+Scores!V4</f>
         <v>2</v>
       </c>
-      <c r="N3" s="2">
+      <c r="N4" s="2">
         <f>Scores!U4+Scores!V4</f>
         <v>3</v>
       </c>
-      <c r="O3" s="2">
-        <f>IF(M3&gt;N3,M3,N3)</f>
-        <v>3</v>
-      </c>
-      <c r="P3" s="5">
-        <f>IF(B3=0," ",IF(B3=Extra!$S$2,VLOOKUP(C3,Extra!$R$4:$AD$8,O3+1),IF(B3=Extra!$W$2,VLOOKUP(C3,Extra!$R$4:$AD$8,(O3+5)),IF(B3=Extra!$AA$2,VLOOKUP(C3,Extra!$R$4:$AD$8,(O3+9)),0))))</f>
-        <v>8</v>
-      </c>
-      <c r="Q3" s="5">
-        <f>IF(I3=0," ",IF(I3=Extra!$S$10,VLOOKUP(F3,Extra!$R$12:$X$17,L3+1),IF(I3=Extra!$V$10,VLOOKUP(F3,Extra!$R$12:$X$17,(L3+4)),0)))</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A4" s="106">
-        <f>Angles!A5</f>
-        <v>3</v>
-      </c>
-      <c r="B4" s="2">
-        <f>IF(A4=0,0,IF(Scores!B5+Scores!C5+Scores!D5=1,1,IF(Scores!B5+Scores!C5+Scores!D5=2,2,IF(Scores!B5+Scores!C5+Scores!D5&gt;=3,3,0))))</f>
-        <v>3</v>
-      </c>
-      <c r="C4" s="2">
-        <f>Scores!E5+Scores!F5+Scores!G5</f>
-        <v>4</v>
-      </c>
-      <c r="D4" s="2">
-        <f>Scores!H5+Scores!I5</f>
-        <v>4</v>
-      </c>
-      <c r="E4" s="2">
-        <f>Scores!J5+Scores!K5</f>
-        <v>2</v>
-      </c>
-      <c r="F4" s="2">
-        <f>IF(D4&gt;E4,D4,E4)</f>
-        <v>4</v>
-      </c>
-      <c r="G4" s="2">
-        <f>Scores!L5</f>
-        <v>1</v>
-      </c>
-      <c r="H4" s="2">
-        <f>Scores!N5</f>
-        <v>1</v>
-      </c>
-      <c r="I4" s="2">
-        <f>IF(A4=0,0,IF(G4&gt;H4,G4,H4))</f>
-        <v>1</v>
-      </c>
-      <c r="J4" s="2">
-        <f>Scores!P5+MAX(Scores!Q5,Scores!M5)</f>
-        <v>1</v>
-      </c>
-      <c r="K4" s="2">
-        <f>Scores!R5+MAX(Scores!S5,Scores!O5)</f>
-        <v>2</v>
-      </c>
-      <c r="L4" s="2">
-        <f>IF(J4&gt;K4,J4,K4)</f>
-        <v>2</v>
-      </c>
-      <c r="M4" s="2">
-        <f>Scores!T5+Scores!V5</f>
-        <v>2</v>
-      </c>
-      <c r="N4" s="2">
-        <f>Scores!U5+Scores!V5</f>
-        <v>3</v>
-      </c>
       <c r="O4" s="2">
-        <f>IF(M4&gt;N4,M4,N4)</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="P4" s="5">
@@ -27445,68 +27399,72 @@
       </c>
       <c r="Q4" s="5">
         <f>IF(I4=0," ",IF(I4=Extra!$S$10,VLOOKUP(F4,Extra!$R$12:$X$17,L4+1),IF(I4=Extra!$V$10,VLOOKUP(F4,Extra!$R$12:$X$17,(L4+4)),0)))</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.45">
+        <v>6</v>
+      </c>
+      <c r="T4"/>
+      <c r="U4"/>
+      <c r="V4"/>
+      <c r="W4"/>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A5" s="106">
-        <f>Angles!A6</f>
+        <f>Angles!A5</f>
+        <v>3</v>
+      </c>
+      <c r="B5" s="2">
+        <f>IF(A5=0,0,IF(Scores!B5+Scores!C5+Scores!D5=1,1,IF(Scores!B5+Scores!C5+Scores!D5=2,2,IF(Scores!B5+Scores!C5+Scores!D5&gt;=3,3,0))))</f>
+        <v>3</v>
+      </c>
+      <c r="C5" s="2">
+        <f>Scores!E5+Scores!F5+Scores!G5</f>
         <v>4</v>
       </c>
-      <c r="B5" s="2">
-        <f>IF(A5=0,0,IF(Scores!B6+Scores!C6+Scores!D6=1,1,IF(Scores!B6+Scores!C6+Scores!D6=2,2,IF(Scores!B6+Scores!C6+Scores!D6&gt;=3,3,0))))</f>
+      <c r="D5" s="2">
+        <f>Scores!H5+Scores!I5</f>
+        <v>4</v>
+      </c>
+      <c r="E5" s="2">
+        <f>Scores!J5+Scores!K5</f>
+        <v>2</v>
+      </c>
+      <c r="F5" s="2">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G5" s="2">
+        <f>Scores!L5</f>
+        <v>1</v>
+      </c>
+      <c r="H5" s="2">
+        <f>Scores!N5</f>
+        <v>1</v>
+      </c>
+      <c r="I5" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J5" s="2">
+        <f>Scores!P5+MAX(Scores!Q5,Scores!M5)</f>
+        <v>1</v>
+      </c>
+      <c r="K5" s="2">
+        <f>Scores!R5+MAX(Scores!S5,Scores!O5)</f>
+        <v>2</v>
+      </c>
+      <c r="L5" s="2">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="M5" s="2">
+        <f>Scores!T5+Scores!V5</f>
+        <v>2</v>
+      </c>
+      <c r="N5" s="2">
+        <f>Scores!U5+Scores!V5</f>
         <v>3</v>
       </c>
-      <c r="C5" s="2">
-        <f>Scores!E6+Scores!F6+Scores!G6</f>
-        <v>4</v>
-      </c>
-      <c r="D5" s="2">
-        <f>Scores!H6+Scores!I6</f>
-        <v>4</v>
-      </c>
-      <c r="E5" s="2">
-        <f>Scores!J6+Scores!K6</f>
-        <v>2</v>
-      </c>
-      <c r="F5" s="2">
-        <f>IF(D5&gt;E5,D5,E5)</f>
-        <v>4</v>
-      </c>
-      <c r="G5" s="2">
-        <f>Scores!L6</f>
-        <v>1</v>
-      </c>
-      <c r="H5" s="2">
-        <f>Scores!N6</f>
-        <v>1</v>
-      </c>
-      <c r="I5" s="2">
-        <f>IF(A5=0,0,IF(G5&gt;H5,G5,H5))</f>
-        <v>1</v>
-      </c>
-      <c r="J5" s="2">
-        <f>Scores!P6+MAX(Scores!Q6,Scores!M6)</f>
-        <v>1</v>
-      </c>
-      <c r="K5" s="2">
-        <f>Scores!R6+MAX(Scores!S6,Scores!O6)</f>
-        <v>2</v>
-      </c>
-      <c r="L5" s="2">
-        <f>IF(J5&gt;K5,J5,K5)</f>
-        <v>2</v>
-      </c>
-      <c r="M5" s="2">
-        <f>Scores!T6+Scores!V6</f>
-        <v>2</v>
-      </c>
-      <c r="N5" s="2">
-        <f>Scores!U6+Scores!V6</f>
-        <v>3</v>
-      </c>
       <c r="O5" s="2">
-        <f>IF(M5&gt;N5,M5,N5)</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="P5" s="5">
@@ -27517,206 +27475,214 @@
         <f>IF(I5=0," ",IF(I5=Extra!$S$10,VLOOKUP(F5,Extra!$R$12:$X$17,L5+1),IF(I5=Extra!$V$10,VLOOKUP(F5,Extra!$R$12:$X$17,(L5+4)),0)))</f>
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="T5"/>
+      <c r="U5"/>
+      <c r="V5"/>
+      <c r="W5"/>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A6" s="106">
-        <f>Angles!A7</f>
-        <v>5</v>
+        <f>Angles!A6</f>
+        <v>4</v>
       </c>
       <c r="B6" s="2">
-        <f>IF(A6=0,0,IF(Scores!B7+Scores!C7+Scores!D7=1,1,IF(Scores!B7+Scores!C7+Scores!D7=2,2,IF(Scores!B7+Scores!C7+Scores!D7&gt;=3,3,0))))</f>
+        <f>IF(A6=0,0,IF(Scores!B6+Scores!C6+Scores!D6=1,1,IF(Scores!B6+Scores!C6+Scores!D6=2,2,IF(Scores!B6+Scores!C6+Scores!D6&gt;=3,3,0))))</f>
         <v>3</v>
       </c>
       <c r="C6" s="2">
-        <f>Scores!E7+Scores!F7+Scores!G7</f>
+        <f>Scores!E6+Scores!F6+Scores!G6</f>
         <v>4</v>
       </c>
       <c r="D6" s="2">
-        <f>Scores!H7+Scores!I7</f>
+        <f>Scores!H6+Scores!I6</f>
         <v>4</v>
       </c>
       <c r="E6" s="2">
-        <f>Scores!J7+Scores!K7</f>
+        <f>Scores!J6+Scores!K6</f>
         <v>2</v>
       </c>
       <c r="F6" s="2">
-        <f>IF(D6&gt;E6,D6,E6)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="G6" s="2">
-        <f>Scores!L7</f>
+        <f>Scores!L6</f>
         <v>1</v>
       </c>
       <c r="H6" s="2">
-        <f>Scores!N7</f>
+        <f>Scores!N6</f>
         <v>1</v>
       </c>
       <c r="I6" s="2">
-        <f>IF(A6=0,0,IF(G6&gt;H6,G6,H6))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J6" s="2">
-        <f>Scores!P7+MAX(Scores!Q7,Scores!M7)</f>
+        <f>Scores!P6+MAX(Scores!Q6,Scores!M6)</f>
         <v>1</v>
       </c>
       <c r="K6" s="2">
-        <f>Scores!R7+MAX(Scores!S7,Scores!O7)</f>
+        <f>Scores!R6+MAX(Scores!S6,Scores!O6)</f>
         <v>2</v>
       </c>
       <c r="L6" s="2">
-        <f>IF(J6&gt;K6,J6,K6)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="M6" s="2">
-        <f>Scores!T7+Scores!V7</f>
-        <v>1</v>
+        <f>Scores!T6+Scores!V6</f>
+        <v>2</v>
       </c>
       <c r="N6" s="2">
-        <f>Scores!U7+Scores!V7</f>
-        <v>2</v>
+        <f>Scores!U6+Scores!V6</f>
+        <v>3</v>
       </c>
       <c r="O6" s="2">
-        <f>IF(M6&gt;N6,M6,N6)</f>
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>3</v>
       </c>
       <c r="P6" s="5">
         <f>IF(B6=0," ",IF(B6=Extra!$S$2,VLOOKUP(C6,Extra!$R$4:$AD$8,O6+1),IF(B6=Extra!$W$2,VLOOKUP(C6,Extra!$R$4:$AD$8,(O6+5)),IF(B6=Extra!$AA$2,VLOOKUP(C6,Extra!$R$4:$AD$8,(O6+9)),0))))</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="Q6" s="5">
         <f>IF(I6=0," ",IF(I6=Extra!$S$10,VLOOKUP(F6,Extra!$R$12:$X$17,L6+1),IF(I6=Extra!$V$10,VLOOKUP(F6,Extra!$R$12:$X$17,(L6+4)),0)))</f>
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="T6"/>
+      <c r="U6"/>
+      <c r="V6"/>
+      <c r="W6"/>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A7" s="106">
+        <f>Angles!A7</f>
+        <v>5</v>
+      </c>
+      <c r="B7" s="2">
+        <f>IF(A7=0,0,IF(Scores!B7+Scores!C7+Scores!D7=1,1,IF(Scores!B7+Scores!C7+Scores!D7=2,2,IF(Scores!B7+Scores!C7+Scores!D7&gt;=3,3,0))))</f>
+        <v>3</v>
+      </c>
+      <c r="C7" s="2">
+        <f>Scores!E7+Scores!F7+Scores!G7</f>
+        <v>4</v>
+      </c>
+      <c r="D7" s="2">
+        <f>Scores!H7+Scores!I7</f>
+        <v>4</v>
+      </c>
+      <c r="E7" s="2">
+        <f>Scores!J7+Scores!K7</f>
+        <v>2</v>
+      </c>
+      <c r="F7" s="2">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G7" s="2">
+        <f>Scores!L7</f>
+        <v>1</v>
+      </c>
+      <c r="H7" s="2">
+        <f>Scores!N7</f>
+        <v>1</v>
+      </c>
+      <c r="I7" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J7" s="2">
+        <f>Scores!P7+MAX(Scores!Q7,Scores!M7)</f>
+        <v>1</v>
+      </c>
+      <c r="K7" s="2">
+        <f>Scores!R7+MAX(Scores!S7,Scores!O7)</f>
+        <v>2</v>
+      </c>
+      <c r="L7" s="2">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="M7" s="2">
+        <f>Scores!T7+Scores!V7</f>
+        <v>1</v>
+      </c>
+      <c r="N7" s="2">
+        <f>Scores!U7+Scores!V7</f>
+        <v>2</v>
+      </c>
+      <c r="O7" s="2">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="P7" s="5">
+        <f>IF(B7=0," ",IF(B7=Extra!$S$2,VLOOKUP(C7,Extra!$R$4:$AD$8,O7+1),IF(B7=Extra!$W$2,VLOOKUP(C7,Extra!$R$4:$AD$8,(O7+5)),IF(B7=Extra!$AA$2,VLOOKUP(C7,Extra!$R$4:$AD$8,(O7+9)),0))))</f>
+        <v>7</v>
+      </c>
+      <c r="Q7" s="5">
+        <f>IF(I7=0," ",IF(I7=Extra!$S$10,VLOOKUP(F7,Extra!$R$12:$X$17,L7+1),IF(I7=Extra!$V$10,VLOOKUP(F7,Extra!$R$12:$X$17,(L7+4)),0)))</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A8" s="106">
         <f>Angles!A8</f>
         <v>6</v>
       </c>
-      <c r="B7" s="2">
-        <f>IF(A7=0,0,IF(Scores!B8+Scores!C8+Scores!D8=1,1,IF(Scores!B8+Scores!C8+Scores!D8=2,2,IF(Scores!B8+Scores!C8+Scores!D8&gt;=3,3,0))))</f>
+      <c r="B8" s="2">
+        <f>IF(A8=0,0,IF(Scores!B8+Scores!C8+Scores!D8=1,1,IF(Scores!B8+Scores!C8+Scores!D8=2,2,IF(Scores!B8+Scores!C8+Scores!D8&gt;=3,3,0))))</f>
         <v>3</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C8" s="2">
         <f>Scores!E8+Scores!F8+Scores!G8</f>
         <v>2</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D8" s="2">
         <f>Scores!H8+Scores!I8</f>
         <v>1</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E8" s="2">
         <f>Scores!J8+Scores!K8</f>
         <v>2</v>
       </c>
-      <c r="F7" s="2">
-        <f>IF(D7&gt;E7,D7,E7)</f>
-        <v>2</v>
-      </c>
-      <c r="G7" s="2">
+      <c r="F8" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G8" s="2">
         <f>Scores!L8</f>
         <v>1</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H8" s="2">
         <f>Scores!N8</f>
         <v>1</v>
       </c>
-      <c r="I7" s="2">
-        <f>IF(A7=0,0,IF(G7&gt;H7,G7,H7))</f>
-        <v>1</v>
-      </c>
-      <c r="J7" s="2">
+      <c r="I8" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J8" s="2">
         <f>Scores!P8+MAX(Scores!Q8,Scores!M8)</f>
         <v>2</v>
       </c>
-      <c r="K7" s="2">
+      <c r="K8" s="2">
         <f>Scores!R8+MAX(Scores!S8,Scores!O8)</f>
         <v>2</v>
       </c>
-      <c r="L7" s="2">
-        <f>IF(J7&gt;K7,J7,K7)</f>
-        <v>2</v>
-      </c>
-      <c r="M7" s="2">
+      <c r="L8" s="2">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="M8" s="2">
         <f>Scores!T8+Scores!V8</f>
         <v>1</v>
       </c>
-      <c r="N7" s="2">
+      <c r="N8" s="2">
         <f>Scores!U8+Scores!V8</f>
         <v>2</v>
       </c>
-      <c r="O7" s="2">
-        <f>IF(M7&gt;N7,M7,N7)</f>
-        <v>2</v>
-      </c>
-      <c r="P7" s="5">
-        <f>IF(B7=0," ",IF(B7=Extra!$S$2,VLOOKUP(C7,Extra!$R$4:$AD$8,O7+1),IF(B7=Extra!$W$2,VLOOKUP(C7,Extra!$R$4:$AD$8,(O7+5)),IF(B7=Extra!$AA$2,VLOOKUP(C7,Extra!$R$4:$AD$8,(O7+9)),0))))</f>
-        <v>5</v>
-      </c>
-      <c r="Q7" s="5">
-        <f>IF(I7=0," ",IF(I7=Extra!$S$10,VLOOKUP(F7,Extra!$R$12:$X$17,L7+1),IF(I7=Extra!$V$10,VLOOKUP(F7,Extra!$R$12:$X$17,(L7+4)),0)))</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A8" s="106">
-        <f>Angles!A9</f>
-        <v>7</v>
-      </c>
-      <c r="B8" s="2">
-        <f>IF(A8=0,0,IF(Scores!B9+Scores!C9+Scores!D9=1,1,IF(Scores!B9+Scores!C9+Scores!D9=2,2,IF(Scores!B9+Scores!C9+Scores!D9&gt;=3,3,0))))</f>
-        <v>3</v>
-      </c>
-      <c r="C8" s="2">
-        <f>Scores!E9+Scores!F9+Scores!G9</f>
-        <v>2</v>
-      </c>
-      <c r="D8" s="2">
-        <f>Scores!H9+Scores!I9</f>
-        <v>1</v>
-      </c>
-      <c r="E8" s="2">
-        <f>Scores!J9+Scores!K9</f>
-        <v>2</v>
-      </c>
-      <c r="F8" s="2">
-        <f>IF(D8&gt;E8,D8,E8)</f>
-        <v>2</v>
-      </c>
-      <c r="G8" s="2">
-        <f>Scores!L9</f>
-        <v>1</v>
-      </c>
-      <c r="H8" s="2">
-        <f>Scores!N9</f>
-        <v>1</v>
-      </c>
-      <c r="I8" s="2">
-        <f>IF(A8=0,0,IF(G8&gt;H8,G8,H8))</f>
-        <v>1</v>
-      </c>
-      <c r="J8" s="2">
-        <f>Scores!P9+MAX(Scores!Q9,Scores!M9)</f>
-        <v>2</v>
-      </c>
-      <c r="K8" s="2">
-        <f>Scores!R9+MAX(Scores!S9,Scores!O9)</f>
-        <v>2</v>
-      </c>
-      <c r="L8" s="2">
-        <f>IF(J8&gt;K8,J8,K8)</f>
-        <v>2</v>
-      </c>
-      <c r="M8" s="2">
-        <f>Scores!T9+Scores!V9</f>
-        <v>1</v>
-      </c>
-      <c r="N8" s="2">
-        <f>Scores!U9+Scores!V9</f>
-        <v>2</v>
-      </c>
       <c r="O8" s="2">
-        <f>IF(M8&gt;N8,M8,N8)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="P8" s="5">
@@ -27728,65 +27694,65 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A9" s="106">
-        <f>Angles!A10</f>
-        <v>8</v>
+        <f>Angles!A9</f>
+        <v>7</v>
       </c>
       <c r="B9" s="2">
-        <f>IF(A9=0,0,IF(Scores!B10+Scores!C10+Scores!D10=1,1,IF(Scores!B10+Scores!C10+Scores!D10=2,2,IF(Scores!B10+Scores!C10+Scores!D10&gt;=3,3,0))))</f>
+        <f>IF(A9=0,0,IF(Scores!B9+Scores!C9+Scores!D9=1,1,IF(Scores!B9+Scores!C9+Scores!D9=2,2,IF(Scores!B9+Scores!C9+Scores!D9&gt;=3,3,0))))</f>
         <v>3</v>
       </c>
       <c r="C9" s="2">
-        <f>Scores!E10+Scores!F10+Scores!G10</f>
+        <f>Scores!E9+Scores!F9+Scores!G9</f>
         <v>2</v>
       </c>
       <c r="D9" s="2">
-        <f>Scores!H10+Scores!I10</f>
+        <f>Scores!H9+Scores!I9</f>
         <v>1</v>
       </c>
       <c r="E9" s="2">
-        <f>Scores!J10+Scores!K10</f>
+        <f>Scores!J9+Scores!K9</f>
         <v>2</v>
       </c>
       <c r="F9" s="2">
-        <f>IF(D9&gt;E9,D9,E9)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="G9" s="2">
-        <f>Scores!L10</f>
+        <f>Scores!L9</f>
         <v>1</v>
       </c>
       <c r="H9" s="2">
-        <f>Scores!N10</f>
+        <f>Scores!N9</f>
         <v>1</v>
       </c>
       <c r="I9" s="2">
-        <f>IF(A9=0,0,IF(G9&gt;H9,G9,H9))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J9" s="2">
-        <f>Scores!P10+MAX(Scores!Q10,Scores!M10)</f>
+        <f>Scores!P9+MAX(Scores!Q9,Scores!M9)</f>
         <v>2</v>
       </c>
       <c r="K9" s="2">
-        <f>Scores!R10+MAX(Scores!S10,Scores!O10)</f>
+        <f>Scores!R9+MAX(Scores!S9,Scores!O9)</f>
         <v>2</v>
       </c>
       <c r="L9" s="2">
-        <f>IF(J9&gt;K9,J9,K9)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="M9" s="2">
-        <f>Scores!T10+Scores!V10</f>
+        <f>Scores!T9+Scores!V9</f>
         <v>1</v>
       </c>
       <c r="N9" s="2">
-        <f>Scores!U10+Scores!V10</f>
+        <f>Scores!U9+Scores!V9</f>
         <v>2</v>
       </c>
       <c r="O9" s="2">
-        <f>IF(M9&gt;N9,M9,N9)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="P9" s="5">
@@ -27798,65 +27764,65 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A10" s="106">
-        <f>Angles!A11</f>
-        <v>9</v>
+        <f>Angles!A10</f>
+        <v>8</v>
       </c>
       <c r="B10" s="2">
-        <f>IF(A10=0,0,IF(Scores!B11+Scores!C11+Scores!D11=1,1,IF(Scores!B11+Scores!C11+Scores!D11=2,2,IF(Scores!B11+Scores!C11+Scores!D11&gt;=3,3,0))))</f>
+        <f>IF(A10=0,0,IF(Scores!B10+Scores!C10+Scores!D10=1,1,IF(Scores!B10+Scores!C10+Scores!D10=2,2,IF(Scores!B10+Scores!C10+Scores!D10&gt;=3,3,0))))</f>
         <v>3</v>
       </c>
       <c r="C10" s="2">
-        <f>Scores!E11+Scores!F11+Scores!G11</f>
+        <f>Scores!E10+Scores!F10+Scores!G10</f>
         <v>2</v>
       </c>
       <c r="D10" s="2">
-        <f>Scores!H11+Scores!I11</f>
+        <f>Scores!H10+Scores!I10</f>
         <v>1</v>
       </c>
       <c r="E10" s="2">
-        <f>Scores!J11+Scores!K11</f>
+        <f>Scores!J10+Scores!K10</f>
         <v>2</v>
       </c>
       <c r="F10" s="2">
-        <f>IF(D10&gt;E10,D10,E10)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="G10" s="2">
-        <f>Scores!L11</f>
+        <f>Scores!L10</f>
         <v>1</v>
       </c>
       <c r="H10" s="2">
-        <f>Scores!N11</f>
+        <f>Scores!N10</f>
         <v>1</v>
       </c>
       <c r="I10" s="2">
-        <f>IF(A10=0,0,IF(G10&gt;H10,G10,H10))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J10" s="2">
-        <f>Scores!P11+MAX(Scores!Q11,Scores!M11)</f>
+        <f>Scores!P10+MAX(Scores!Q10,Scores!M10)</f>
         <v>2</v>
       </c>
       <c r="K10" s="2">
-        <f>Scores!R11+MAX(Scores!S11,Scores!O11)</f>
+        <f>Scores!R10+MAX(Scores!S10,Scores!O10)</f>
         <v>2</v>
       </c>
       <c r="L10" s="2">
-        <f>IF(J10&gt;K10,J10,K10)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="M10" s="2">
-        <f>Scores!T11+Scores!V11</f>
+        <f>Scores!T10+Scores!V10</f>
         <v>1</v>
       </c>
       <c r="N10" s="2">
-        <f>Scores!U11+Scores!V11</f>
+        <f>Scores!U10+Scores!V10</f>
         <v>2</v>
       </c>
       <c r="O10" s="2">
-        <f>IF(M10&gt;N10,M10,N10)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="P10" s="5">
@@ -27868,135 +27834,135 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A11" s="106">
+        <f>Angles!A11</f>
+        <v>9</v>
+      </c>
+      <c r="B11" s="2">
+        <f>IF(A11=0,0,IF(Scores!B11+Scores!C11+Scores!D11=1,1,IF(Scores!B11+Scores!C11+Scores!D11=2,2,IF(Scores!B11+Scores!C11+Scores!D11&gt;=3,3,0))))</f>
+        <v>3</v>
+      </c>
+      <c r="C11" s="2">
+        <f>Scores!E11+Scores!F11+Scores!G11</f>
+        <v>2</v>
+      </c>
+      <c r="D11" s="2">
+        <f>Scores!H11+Scores!I11</f>
+        <v>1</v>
+      </c>
+      <c r="E11" s="2">
+        <f>Scores!J11+Scores!K11</f>
+        <v>2</v>
+      </c>
+      <c r="F11" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G11" s="2">
+        <f>Scores!L11</f>
+        <v>1</v>
+      </c>
+      <c r="H11" s="2">
+        <f>Scores!N11</f>
+        <v>1</v>
+      </c>
+      <c r="I11" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J11" s="2">
+        <f>Scores!P11+MAX(Scores!Q11,Scores!M11)</f>
+        <v>2</v>
+      </c>
+      <c r="K11" s="2">
+        <f>Scores!R11+MAX(Scores!S11,Scores!O11)</f>
+        <v>2</v>
+      </c>
+      <c r="L11" s="2">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="M11" s="2">
+        <f>Scores!T11+Scores!V11</f>
+        <v>1</v>
+      </c>
+      <c r="N11" s="2">
+        <f>Scores!U11+Scores!V11</f>
+        <v>2</v>
+      </c>
+      <c r="O11" s="2">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="P11" s="5">
+        <f>IF(B11=0," ",IF(B11=Extra!$S$2,VLOOKUP(C11,Extra!$R$4:$AD$8,O11+1),IF(B11=Extra!$W$2,VLOOKUP(C11,Extra!$R$4:$AD$8,(O11+5)),IF(B11=Extra!$AA$2,VLOOKUP(C11,Extra!$R$4:$AD$8,(O11+9)),0))))</f>
+        <v>5</v>
+      </c>
+      <c r="Q11" s="5">
+        <f>IF(I11=0," ",IF(I11=Extra!$S$10,VLOOKUP(F11,Extra!$R$12:$X$17,L11+1),IF(I11=Extra!$V$10,VLOOKUP(F11,Extra!$R$12:$X$17,(L11+4)),0)))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A12" s="106">
         <f>Angles!A12</f>
         <v>10</v>
       </c>
-      <c r="B11" s="2">
-        <f>IF(A11=0,0,IF(Scores!B12+Scores!C12+Scores!D12=1,1,IF(Scores!B12+Scores!C12+Scores!D12=2,2,IF(Scores!B12+Scores!C12+Scores!D12&gt;=3,3,0))))</f>
+      <c r="B12" s="2">
+        <f>IF(A12=0,0,IF(Scores!B12+Scores!C12+Scores!D12=1,1,IF(Scores!B12+Scores!C12+Scores!D12=2,2,IF(Scores!B12+Scores!C12+Scores!D12&gt;=3,3,0))))</f>
         <v>3</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C12" s="2">
         <f>Scores!E12+Scores!F12+Scores!G12</f>
         <v>1</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D12" s="2">
         <f>Scores!H12+Scores!I12</f>
         <v>1</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E12" s="2">
         <f>Scores!J12+Scores!K12</f>
         <v>2</v>
       </c>
-      <c r="F11" s="2">
-        <f>IF(D11&gt;E11,D11,E11)</f>
-        <v>2</v>
-      </c>
-      <c r="G11" s="2">
+      <c r="F12" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G12" s="2">
         <f>Scores!L12</f>
         <v>1</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H12" s="2">
         <f>Scores!N12</f>
         <v>1</v>
       </c>
-      <c r="I11" s="2">
-        <f>IF(A11=0,0,IF(G11&gt;H11,G11,H11))</f>
-        <v>1</v>
-      </c>
-      <c r="J11" s="2">
+      <c r="I12" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J12" s="2">
         <f>Scores!P12+MAX(Scores!Q12,Scores!M12)</f>
         <v>2</v>
       </c>
-      <c r="K11" s="2">
+      <c r="K12" s="2">
         <f>Scores!R12+MAX(Scores!S12,Scores!O12)</f>
         <v>2</v>
       </c>
-      <c r="L11" s="2">
-        <f>IF(J11&gt;K11,J11,K11)</f>
-        <v>2</v>
-      </c>
-      <c r="M11" s="2">
+      <c r="L12" s="2">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="M12" s="2">
         <f>Scores!T12+Scores!V12</f>
         <v>1</v>
       </c>
-      <c r="N11" s="2">
+      <c r="N12" s="2">
         <f>Scores!U12+Scores!V12</f>
         <v>2</v>
       </c>
-      <c r="O11" s="2">
-        <f>IF(M11&gt;N11,M11,N11)</f>
-        <v>2</v>
-      </c>
-      <c r="P11" s="5">
-        <f>IF(B11=0," ",IF(B11=Extra!$S$2,VLOOKUP(C11,Extra!$R$4:$AD$8,O11+1),IF(B11=Extra!$W$2,VLOOKUP(C11,Extra!$R$4:$AD$8,(O11+5)),IF(B11=Extra!$AA$2,VLOOKUP(C11,Extra!$R$4:$AD$8,(O11+9)),0))))</f>
-        <v>3</v>
-      </c>
-      <c r="Q11" s="5">
-        <f>IF(I11=0," ",IF(I11=Extra!$S$10,VLOOKUP(F11,Extra!$R$12:$X$17,L11+1),IF(I11=Extra!$V$10,VLOOKUP(F11,Extra!$R$12:$X$17,(L11+4)),0)))</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A12" s="106">
-        <f>Angles!A13</f>
-        <v>11</v>
-      </c>
-      <c r="B12" s="2">
-        <f>IF(A12=0,0,IF(Scores!B13+Scores!C13+Scores!D13=1,1,IF(Scores!B13+Scores!C13+Scores!D13=2,2,IF(Scores!B13+Scores!C13+Scores!D13&gt;=3,3,0))))</f>
-        <v>3</v>
-      </c>
-      <c r="C12" s="2">
-        <f>Scores!E13+Scores!F13+Scores!G13</f>
-        <v>1</v>
-      </c>
-      <c r="D12" s="2">
-        <f>Scores!H13+Scores!I13</f>
-        <v>1</v>
-      </c>
-      <c r="E12" s="2">
-        <f>Scores!J13+Scores!K13</f>
-        <v>2</v>
-      </c>
-      <c r="F12" s="2">
-        <f>IF(D12&gt;E12,D12,E12)</f>
-        <v>2</v>
-      </c>
-      <c r="G12" s="2">
-        <f>Scores!L13</f>
-        <v>1</v>
-      </c>
-      <c r="H12" s="2">
-        <f>Scores!N13</f>
-        <v>1</v>
-      </c>
-      <c r="I12" s="2">
-        <f>IF(A12=0,0,IF(G12&gt;H12,G12,H12))</f>
-        <v>1</v>
-      </c>
-      <c r="J12" s="2">
-        <f>Scores!P13+MAX(Scores!Q13,Scores!M13)</f>
-        <v>2</v>
-      </c>
-      <c r="K12" s="2">
-        <f>Scores!R13+MAX(Scores!S13,Scores!O13)</f>
-        <v>2</v>
-      </c>
-      <c r="L12" s="2">
-        <f>IF(J12&gt;K12,J12,K12)</f>
-        <v>2</v>
-      </c>
-      <c r="M12" s="2">
-        <f>Scores!T13+Scores!V13</f>
-        <v>1</v>
-      </c>
-      <c r="N12" s="2">
-        <f>Scores!U13+Scores!V13</f>
-        <v>2</v>
-      </c>
       <c r="O12" s="2">
-        <f>IF(M12&gt;N12,M12,N12)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="P12" s="5">
@@ -28008,555 +27974,555 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A13" s="106">
+        <f>Angles!A13</f>
+        <v>11</v>
+      </c>
+      <c r="B13" s="2">
+        <f>IF(A13=0,0,IF(Scores!B13+Scores!C13+Scores!D13=1,1,IF(Scores!B13+Scores!C13+Scores!D13=2,2,IF(Scores!B13+Scores!C13+Scores!D13&gt;=3,3,0))))</f>
+        <v>3</v>
+      </c>
+      <c r="C13" s="2">
+        <f>Scores!E13+Scores!F13+Scores!G13</f>
+        <v>1</v>
+      </c>
+      <c r="D13" s="2">
+        <f>Scores!H13+Scores!I13</f>
+        <v>1</v>
+      </c>
+      <c r="E13" s="2">
+        <f>Scores!J13+Scores!K13</f>
+        <v>2</v>
+      </c>
+      <c r="F13" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G13" s="2">
+        <f>Scores!L13</f>
+        <v>1</v>
+      </c>
+      <c r="H13" s="2">
+        <f>Scores!N13</f>
+        <v>1</v>
+      </c>
+      <c r="I13" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J13" s="2">
+        <f>Scores!P13+MAX(Scores!Q13,Scores!M13)</f>
+        <v>2</v>
+      </c>
+      <c r="K13" s="2">
+        <f>Scores!R13+MAX(Scores!S13,Scores!O13)</f>
+        <v>2</v>
+      </c>
+      <c r="L13" s="2">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="M13" s="2">
+        <f>Scores!T13+Scores!V13</f>
+        <v>1</v>
+      </c>
+      <c r="N13" s="2">
+        <f>Scores!U13+Scores!V13</f>
+        <v>2</v>
+      </c>
+      <c r="O13" s="2">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="P13" s="5">
+        <f>IF(B13=0," ",IF(B13=Extra!$S$2,VLOOKUP(C13,Extra!$R$4:$AD$8,O13+1),IF(B13=Extra!$W$2,VLOOKUP(C13,Extra!$R$4:$AD$8,(O13+5)),IF(B13=Extra!$AA$2,VLOOKUP(C13,Extra!$R$4:$AD$8,(O13+9)),0))))</f>
+        <v>3</v>
+      </c>
+      <c r="Q13" s="5">
+        <f>IF(I13=0," ",IF(I13=Extra!$S$10,VLOOKUP(F13,Extra!$R$12:$X$17,L13+1),IF(I13=Extra!$V$10,VLOOKUP(F13,Extra!$R$12:$X$17,(L13+4)),0)))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A14" s="106">
         <f>Angles!A14</f>
         <v>12</v>
       </c>
-      <c r="B13" s="2">
-        <f>IF(A13=0,0,IF(Scores!B14+Scores!C14+Scores!D14=1,1,IF(Scores!B14+Scores!C14+Scores!D14=2,2,IF(Scores!B14+Scores!C14+Scores!D14&gt;=3,3,0))))</f>
-        <v>1</v>
-      </c>
-      <c r="C13" s="2">
+      <c r="B14" s="2">
+        <f>IF(A14=0,0,IF(Scores!B14+Scores!C14+Scores!D14=1,1,IF(Scores!B14+Scores!C14+Scores!D14=2,2,IF(Scores!B14+Scores!C14+Scores!D14&gt;=3,3,0))))</f>
+        <v>1</v>
+      </c>
+      <c r="C14" s="2">
         <f>Scores!E14+Scores!F14+Scores!G14</f>
         <v>1</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D14" s="2">
         <f>Scores!H14+Scores!I14</f>
         <v>1</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E14" s="2">
         <f>Scores!J14+Scores!K14</f>
         <v>2</v>
       </c>
-      <c r="F13" s="2">
-        <f>IF(D13&gt;E13,D13,E13)</f>
-        <v>2</v>
-      </c>
-      <c r="G13" s="2">
+      <c r="F14" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G14" s="2">
         <f>Scores!L14</f>
         <v>1</v>
       </c>
-      <c r="H13" s="2">
+      <c r="H14" s="2">
         <f>Scores!N14</f>
         <v>1</v>
       </c>
-      <c r="I13" s="2">
-        <f>IF(A13=0,0,IF(G13&gt;H13,G13,H13))</f>
-        <v>1</v>
-      </c>
-      <c r="J13" s="2">
+      <c r="I14" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J14" s="2">
         <f>Scores!P14+MAX(Scores!Q14,Scores!M14)</f>
         <v>2</v>
       </c>
-      <c r="K13" s="2">
+      <c r="K14" s="2">
         <f>Scores!R14+MAX(Scores!S14,Scores!O14)</f>
         <v>1</v>
       </c>
-      <c r="L13" s="2">
-        <f>IF(J13&gt;K13,J13,K13)</f>
-        <v>2</v>
-      </c>
-      <c r="M13" s="2">
+      <c r="L14" s="2">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="M14" s="2">
         <f>Scores!T14+Scores!V14</f>
         <v>1</v>
       </c>
-      <c r="N13" s="2">
+      <c r="N14" s="2">
         <f>Scores!U14+Scores!V14</f>
         <v>2</v>
       </c>
-      <c r="O13" s="2">
-        <f>IF(M13&gt;N13,M13,N13)</f>
-        <v>2</v>
-      </c>
-      <c r="P13" s="5">
-        <f>IF(B13=0," ",IF(B13=Extra!$S$2,VLOOKUP(C13,Extra!$R$4:$AD$8,O13+1),IF(B13=Extra!$W$2,VLOOKUP(C13,Extra!$R$4:$AD$8,(O13+5)),IF(B13=Extra!$AA$2,VLOOKUP(C13,Extra!$R$4:$AD$8,(O13+9)),0))))</f>
-        <v>2</v>
-      </c>
-      <c r="Q13" s="5">
-        <f>IF(I13=0," ",IF(I13=Extra!$S$10,VLOOKUP(F13,Extra!$R$12:$X$17,L13+1),IF(I13=Extra!$V$10,VLOOKUP(F13,Extra!$R$12:$X$17,(L13+4)),0)))</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A14" s="106">
+      <c r="O14" s="2">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="P14" s="5">
+        <f>IF(B14=0," ",IF(B14=Extra!$S$2,VLOOKUP(C14,Extra!$R$4:$AD$8,O14+1),IF(B14=Extra!$W$2,VLOOKUP(C14,Extra!$R$4:$AD$8,(O14+5)),IF(B14=Extra!$AA$2,VLOOKUP(C14,Extra!$R$4:$AD$8,(O14+9)),0))))</f>
+        <v>2</v>
+      </c>
+      <c r="Q14" s="5">
+        <f>IF(I14=0," ",IF(I14=Extra!$S$10,VLOOKUP(F14,Extra!$R$12:$X$17,L14+1),IF(I14=Extra!$V$10,VLOOKUP(F14,Extra!$R$12:$X$17,(L14+4)),0)))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A15" s="106">
         <f>Angles!A15</f>
         <v>13</v>
       </c>
-      <c r="B14" s="2">
-        <f>IF(A14=0,0,IF(Scores!B15+Scores!C15+Scores!D15=1,1,IF(Scores!B15+Scores!C15+Scores!D15=2,2,IF(Scores!B15+Scores!C15+Scores!D15&gt;=3,3,0))))</f>
-        <v>1</v>
-      </c>
-      <c r="C14" s="2">
+      <c r="B15" s="2">
+        <f>IF(A15=0,0,IF(Scores!B15+Scores!C15+Scores!D15=1,1,IF(Scores!B15+Scores!C15+Scores!D15=2,2,IF(Scores!B15+Scores!C15+Scores!D15&gt;=3,3,0))))</f>
+        <v>1</v>
+      </c>
+      <c r="C15" s="2">
         <f>Scores!E15+Scores!F15+Scores!G15</f>
         <v>1</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D15" s="2">
         <f>Scores!H15+Scores!I15</f>
         <v>1</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E15" s="2">
         <f>Scores!J15+Scores!K15</f>
         <v>2</v>
       </c>
-      <c r="F14" s="2">
-        <f>IF(D14&gt;E14,D14,E14)</f>
-        <v>2</v>
-      </c>
-      <c r="G14" s="2">
+      <c r="F15" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G15" s="2">
         <f>Scores!L15</f>
         <v>1</v>
       </c>
-      <c r="H14" s="2">
+      <c r="H15" s="2">
         <f>Scores!N15</f>
         <v>1</v>
       </c>
-      <c r="I14" s="2">
-        <f>IF(A14=0,0,IF(G14&gt;H14,G14,H14))</f>
-        <v>1</v>
-      </c>
-      <c r="J14" s="2">
+      <c r="I15" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J15" s="2">
         <f>Scores!P15+MAX(Scores!Q15,Scores!M15)</f>
         <v>1</v>
       </c>
-      <c r="K14" s="2">
+      <c r="K15" s="2">
         <f>Scores!R15+MAX(Scores!S15,Scores!O15)</f>
         <v>1</v>
       </c>
-      <c r="L14" s="2">
-        <f>IF(J14&gt;K14,J14,K14)</f>
-        <v>1</v>
-      </c>
-      <c r="M14" s="2">
+      <c r="L15" s="2">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="M15" s="2">
         <f>Scores!T15+Scores!V15</f>
         <v>1</v>
       </c>
-      <c r="N14" s="2">
+      <c r="N15" s="2">
         <f>Scores!U15+Scores!V15</f>
         <v>2</v>
       </c>
-      <c r="O14" s="2">
-        <f>IF(M14&gt;N14,M14,N14)</f>
-        <v>2</v>
-      </c>
-      <c r="P14" s="5">
-        <f>IF(B14=0," ",IF(B14=Extra!$S$2,VLOOKUP(C14,Extra!$R$4:$AD$8,O14+1),IF(B14=Extra!$W$2,VLOOKUP(C14,Extra!$R$4:$AD$8,(O14+5)),IF(B14=Extra!$AA$2,VLOOKUP(C14,Extra!$R$4:$AD$8,(O14+9)),0))))</f>
-        <v>2</v>
-      </c>
-      <c r="Q14" s="5">
-        <f>IF(I14=0," ",IF(I14=Extra!$S$10,VLOOKUP(F14,Extra!$R$12:$X$17,L14+1),IF(I14=Extra!$V$10,VLOOKUP(F14,Extra!$R$12:$X$17,(L14+4)),0)))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A15" s="106">
+      <c r="O15" s="2">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="P15" s="5">
+        <f>IF(B15=0," ",IF(B15=Extra!$S$2,VLOOKUP(C15,Extra!$R$4:$AD$8,O15+1),IF(B15=Extra!$W$2,VLOOKUP(C15,Extra!$R$4:$AD$8,(O15+5)),IF(B15=Extra!$AA$2,VLOOKUP(C15,Extra!$R$4:$AD$8,(O15+9)),0))))</f>
+        <v>2</v>
+      </c>
+      <c r="Q15" s="5">
+        <f>IF(I15=0," ",IF(I15=Extra!$S$10,VLOOKUP(F15,Extra!$R$12:$X$17,L15+1),IF(I15=Extra!$V$10,VLOOKUP(F15,Extra!$R$12:$X$17,(L15+4)),0)))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A16" s="106">
         <f>Angles!A16</f>
         <v>14</v>
       </c>
-      <c r="B15" s="2">
-        <f>IF(A15=0,0,IF(Scores!B16+Scores!C16+Scores!D16=1,1,IF(Scores!B16+Scores!C16+Scores!D16=2,2,IF(Scores!B16+Scores!C16+Scores!D16&gt;=3,3,0))))</f>
-        <v>1</v>
-      </c>
-      <c r="C15" s="2">
+      <c r="B16" s="2">
+        <f>IF(A16=0,0,IF(Scores!B16+Scores!C16+Scores!D16=1,1,IF(Scores!B16+Scores!C16+Scores!D16=2,2,IF(Scores!B16+Scores!C16+Scores!D16&gt;=3,3,0))))</f>
+        <v>1</v>
+      </c>
+      <c r="C16" s="2">
         <f>Scores!E16+Scores!F16+Scores!G16</f>
         <v>1</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D16" s="2">
         <f>Scores!H16+Scores!I16</f>
         <v>1</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E16" s="2">
         <f>Scores!J16+Scores!K16</f>
         <v>2</v>
       </c>
-      <c r="F15" s="2">
-        <f>IF(D15&gt;E15,D15,E15)</f>
-        <v>2</v>
-      </c>
-      <c r="G15" s="2">
+      <c r="F16" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G16" s="2">
         <f>Scores!L16</f>
         <v>1</v>
       </c>
-      <c r="H15" s="2">
+      <c r="H16" s="2">
         <f>Scores!N16</f>
         <v>1</v>
       </c>
-      <c r="I15" s="2">
-        <f>IF(A15=0,0,IF(G15&gt;H15,G15,H15))</f>
-        <v>1</v>
-      </c>
-      <c r="J15" s="2">
+      <c r="I16" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J16" s="2">
         <f>Scores!P16+MAX(Scores!Q16,Scores!M16)</f>
         <v>1</v>
       </c>
-      <c r="K15" s="2">
+      <c r="K16" s="2">
         <f>Scores!R16+MAX(Scores!S16,Scores!O16)</f>
         <v>1</v>
       </c>
-      <c r="L15" s="2">
-        <f>IF(J15&gt;K15,J15,K15)</f>
-        <v>1</v>
-      </c>
-      <c r="M15" s="2">
+      <c r="L16" s="2">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="M16" s="2">
         <f>Scores!T16+Scores!V16</f>
         <v>1</v>
       </c>
-      <c r="N15" s="2">
+      <c r="N16" s="2">
         <f>Scores!U16+Scores!V16</f>
         <v>2</v>
       </c>
-      <c r="O15" s="2">
-        <f>IF(M15&gt;N15,M15,N15)</f>
-        <v>2</v>
-      </c>
-      <c r="P15" s="5">
-        <f>IF(B15=0," ",IF(B15=Extra!$S$2,VLOOKUP(C15,Extra!$R$4:$AD$8,O15+1),IF(B15=Extra!$W$2,VLOOKUP(C15,Extra!$R$4:$AD$8,(O15+5)),IF(B15=Extra!$AA$2,VLOOKUP(C15,Extra!$R$4:$AD$8,(O15+9)),0))))</f>
-        <v>2</v>
-      </c>
-      <c r="Q15" s="5">
-        <f>IF(I15=0," ",IF(I15=Extra!$S$10,VLOOKUP(F15,Extra!$R$12:$X$17,L15+1),IF(I15=Extra!$V$10,VLOOKUP(F15,Extra!$R$12:$X$17,(L15+4)),0)))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A16" s="106">
+      <c r="O16" s="2">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="P16" s="5">
+        <f>IF(B16=0," ",IF(B16=Extra!$S$2,VLOOKUP(C16,Extra!$R$4:$AD$8,O16+1),IF(B16=Extra!$W$2,VLOOKUP(C16,Extra!$R$4:$AD$8,(O16+5)),IF(B16=Extra!$AA$2,VLOOKUP(C16,Extra!$R$4:$AD$8,(O16+9)),0))))</f>
+        <v>2</v>
+      </c>
+      <c r="Q16" s="5">
+        <f>IF(I16=0," ",IF(I16=Extra!$S$10,VLOOKUP(F16,Extra!$R$12:$X$17,L16+1),IF(I16=Extra!$V$10,VLOOKUP(F16,Extra!$R$12:$X$17,(L16+4)),0)))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:31" x14ac:dyDescent="0.45">
+      <c r="A17" s="106">
         <f>Angles!A17</f>
         <v>15</v>
       </c>
-      <c r="B16" s="2">
-        <f>IF(A16=0,0,IF(Scores!B17+Scores!C17+Scores!D17=1,1,IF(Scores!B17+Scores!C17+Scores!D17=2,2,IF(Scores!B17+Scores!C17+Scores!D17&gt;=3,3,0))))</f>
-        <v>1</v>
-      </c>
-      <c r="C16" s="2">
+      <c r="B17" s="2">
+        <f>IF(A17=0,0,IF(Scores!B17+Scores!C17+Scores!D17=1,1,IF(Scores!B17+Scores!C17+Scores!D17=2,2,IF(Scores!B17+Scores!C17+Scores!D17&gt;=3,3,0))))</f>
+        <v>1</v>
+      </c>
+      <c r="C17" s="2">
         <f>Scores!E17+Scores!F17+Scores!G17</f>
         <v>1</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D17" s="2">
         <f>Scores!H17+Scores!I17</f>
         <v>1</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E17" s="2">
         <f>Scores!J17+Scores!K17</f>
         <v>2</v>
       </c>
-      <c r="F16" s="2">
-        <f>IF(D16&gt;E16,D16,E16)</f>
-        <v>2</v>
-      </c>
-      <c r="G16" s="2">
+      <c r="F17" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G17" s="2">
         <f>Scores!L17</f>
         <v>1</v>
       </c>
-      <c r="H16" s="2">
+      <c r="H17" s="2">
         <f>Scores!N17</f>
         <v>1</v>
       </c>
-      <c r="I16" s="2">
-        <f>IF(A16=0,0,IF(G16&gt;H16,G16,H16))</f>
-        <v>1</v>
-      </c>
-      <c r="J16" s="2">
+      <c r="I17" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J17" s="2">
         <f>Scores!P17+MAX(Scores!Q17,Scores!M17)</f>
         <v>1</v>
       </c>
-      <c r="K16" s="2">
+      <c r="K17" s="2">
         <f>Scores!R17+MAX(Scores!S17,Scores!O17)</f>
         <v>1</v>
       </c>
-      <c r="L16" s="2">
-        <f>IF(J16&gt;K16,J16,K16)</f>
-        <v>1</v>
-      </c>
-      <c r="M16" s="2">
+      <c r="L17" s="2">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="M17" s="2">
         <f>Scores!T17+Scores!V17</f>
         <v>1</v>
       </c>
-      <c r="N16" s="2">
+      <c r="N17" s="2">
         <f>Scores!U17+Scores!V17</f>
         <v>2</v>
       </c>
-      <c r="O16" s="2">
-        <f>IF(M16&gt;N16,M16,N16)</f>
-        <v>2</v>
-      </c>
-      <c r="P16" s="5">
-        <f>IF(B16=0," ",IF(B16=Extra!$S$2,VLOOKUP(C16,Extra!$R$4:$AD$8,O16+1),IF(B16=Extra!$W$2,VLOOKUP(C16,Extra!$R$4:$AD$8,(O16+5)),IF(B16=Extra!$AA$2,VLOOKUP(C16,Extra!$R$4:$AD$8,(O16+9)),0))))</f>
-        <v>2</v>
-      </c>
-      <c r="Q16" s="5">
-        <f>IF(I16=0," ",IF(I16=Extra!$S$10,VLOOKUP(F16,Extra!$R$12:$X$17,L16+1),IF(I16=Extra!$V$10,VLOOKUP(F16,Extra!$R$12:$X$17,(L16+4)),0)))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.45">
-      <c r="A17" s="106">
+      <c r="O17" s="2">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="P17" s="5">
+        <f>IF(B17=0," ",IF(B17=Extra!$S$2,VLOOKUP(C17,Extra!$R$4:$AD$8,O17+1),IF(B17=Extra!$W$2,VLOOKUP(C17,Extra!$R$4:$AD$8,(O17+5)),IF(B17=Extra!$AA$2,VLOOKUP(C17,Extra!$R$4:$AD$8,(O17+9)),0))))</f>
+        <v>2</v>
+      </c>
+      <c r="Q17" s="5">
+        <f>IF(I17=0," ",IF(I17=Extra!$S$10,VLOOKUP(F17,Extra!$R$12:$X$17,L17+1),IF(I17=Extra!$V$10,VLOOKUP(F17,Extra!$R$12:$X$17,(L17+4)),0)))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:31" x14ac:dyDescent="0.45">
+      <c r="A18" s="106">
         <f>Angles!A18</f>
         <v>16</v>
       </c>
-      <c r="B17" s="2">
-        <f>IF(A17=0,0,IF(Scores!B18+Scores!C18+Scores!D18=1,1,IF(Scores!B18+Scores!C18+Scores!D18=2,2,IF(Scores!B18+Scores!C18+Scores!D18&gt;=3,3,0))))</f>
-        <v>1</v>
-      </c>
-      <c r="C17" s="2">
+      <c r="B18" s="2">
+        <f>IF(A18=0,0,IF(Scores!B18+Scores!C18+Scores!D18=1,1,IF(Scores!B18+Scores!C18+Scores!D18=2,2,IF(Scores!B18+Scores!C18+Scores!D18&gt;=3,3,0))))</f>
+        <v>1</v>
+      </c>
+      <c r="C18" s="2">
         <f>Scores!E18+Scores!F18+Scores!G18</f>
         <v>1</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D18" s="2">
         <f>Scores!H18+Scores!I18</f>
         <v>1</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E18" s="2">
         <f>Scores!J18+Scores!K18</f>
         <v>2</v>
       </c>
-      <c r="F17" s="2">
-        <f>IF(D17&gt;E17,D17,E17)</f>
-        <v>2</v>
-      </c>
-      <c r="G17" s="2">
+      <c r="F18" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G18" s="2">
         <f>Scores!L18</f>
         <v>1</v>
       </c>
-      <c r="H17" s="2">
+      <c r="H18" s="2">
         <f>Scores!N18</f>
         <v>1</v>
       </c>
-      <c r="I17" s="2">
-        <f>IF(A17=0,0,IF(G17&gt;H17,G17,H17))</f>
-        <v>1</v>
-      </c>
-      <c r="J17" s="2">
+      <c r="I18" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J18" s="2">
         <f>Scores!P18+MAX(Scores!Q18,Scores!M18)</f>
         <v>1</v>
       </c>
-      <c r="K17" s="2">
+      <c r="K18" s="2">
         <f>Scores!R18+MAX(Scores!S18,Scores!O18)</f>
         <v>1</v>
       </c>
-      <c r="L17" s="2">
-        <f>IF(J17&gt;K17,J17,K17)</f>
-        <v>1</v>
-      </c>
-      <c r="M17" s="2">
+      <c r="L18" s="2">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="M18" s="2">
         <f>Scores!T18+Scores!V18</f>
         <v>1</v>
       </c>
-      <c r="N17" s="2">
+      <c r="N18" s="2">
         <f>Scores!U18+Scores!V18</f>
         <v>2</v>
       </c>
-      <c r="O17" s="2">
-        <f>IF(M17&gt;N17,M17,N17)</f>
-        <v>2</v>
-      </c>
-      <c r="P17" s="5">
-        <f>IF(B17=0," ",IF(B17=Extra!$S$2,VLOOKUP(C17,Extra!$R$4:$AD$8,O17+1),IF(B17=Extra!$W$2,VLOOKUP(C17,Extra!$R$4:$AD$8,(O17+5)),IF(B17=Extra!$AA$2,VLOOKUP(C17,Extra!$R$4:$AD$8,(O17+9)),0))))</f>
-        <v>2</v>
-      </c>
-      <c r="Q17" s="5">
-        <f>IF(I17=0," ",IF(I17=Extra!$S$10,VLOOKUP(F17,Extra!$R$12:$X$17,L17+1),IF(I17=Extra!$V$10,VLOOKUP(F17,Extra!$R$12:$X$17,(L17+4)),0)))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.45">
-      <c r="A18" s="106">
+      <c r="O18" s="2">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="P18" s="5">
+        <f>IF(B18=0," ",IF(B18=Extra!$S$2,VLOOKUP(C18,Extra!$R$4:$AD$8,O18+1),IF(B18=Extra!$W$2,VLOOKUP(C18,Extra!$R$4:$AD$8,(O18+5)),IF(B18=Extra!$AA$2,VLOOKUP(C18,Extra!$R$4:$AD$8,(O18+9)),0))))</f>
+        <v>2</v>
+      </c>
+      <c r="Q18" s="5">
+        <f>IF(I18=0," ",IF(I18=Extra!$S$10,VLOOKUP(F18,Extra!$R$12:$X$17,L18+1),IF(I18=Extra!$V$10,VLOOKUP(F18,Extra!$R$12:$X$17,(L18+4)),0)))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:31" x14ac:dyDescent="0.45">
+      <c r="A19" s="106">
         <f>Angles!A19</f>
         <v>17</v>
       </c>
-      <c r="B18" s="2">
-        <f>IF(A18=0,0,IF(Scores!B19+Scores!C19+Scores!D19=1,1,IF(Scores!B19+Scores!C19+Scores!D19=2,2,IF(Scores!B19+Scores!C19+Scores!D19&gt;=3,3,0))))</f>
-        <v>1</v>
-      </c>
-      <c r="C18" s="2">
+      <c r="B19" s="2">
+        <f>IF(A19=0,0,IF(Scores!B19+Scores!C19+Scores!D19=1,1,IF(Scores!B19+Scores!C19+Scores!D19=2,2,IF(Scores!B19+Scores!C19+Scores!D19&gt;=3,3,0))))</f>
+        <v>1</v>
+      </c>
+      <c r="C19" s="2">
         <f>Scores!E19+Scores!F19+Scores!G19</f>
         <v>1</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D19" s="2">
         <f>Scores!H19+Scores!I19</f>
         <v>1</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E19" s="2">
         <f>Scores!J19+Scores!K19</f>
         <v>2</v>
       </c>
-      <c r="F18" s="2">
-        <f>IF(D18&gt;E18,D18,E18)</f>
-        <v>2</v>
-      </c>
-      <c r="G18" s="2">
+      <c r="F19" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G19" s="2">
         <f>Scores!L19</f>
         <v>1</v>
       </c>
-      <c r="H18" s="2">
+      <c r="H19" s="2">
         <f>Scores!N19</f>
         <v>1</v>
       </c>
-      <c r="I18" s="2">
-        <f>IF(A18=0,0,IF(G18&gt;H18,G18,H18))</f>
-        <v>1</v>
-      </c>
-      <c r="J18" s="2">
+      <c r="I19" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J19" s="2">
         <f>Scores!P19+MAX(Scores!Q19,Scores!M19)</f>
         <v>2</v>
       </c>
-      <c r="K18" s="2">
+      <c r="K19" s="2">
         <f>Scores!R19+MAX(Scores!S19,Scores!O19)</f>
         <v>1</v>
       </c>
-      <c r="L18" s="2">
-        <f>IF(J18&gt;K18,J18,K18)</f>
-        <v>2</v>
-      </c>
-      <c r="M18" s="2">
+      <c r="L19" s="2">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="M19" s="2">
         <f>Scores!T19+Scores!V19</f>
         <v>2</v>
       </c>
-      <c r="N18" s="2">
+      <c r="N19" s="2">
         <f>Scores!U19+Scores!V19</f>
         <v>3</v>
       </c>
-      <c r="O18" s="2">
-        <f>IF(M18&gt;N18,M18,N18)</f>
+      <c r="O19" s="2">
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="P18" s="5">
-        <f>IF(B18=0," ",IF(B18=Extra!$S$2,VLOOKUP(C18,Extra!$R$4:$AD$8,O18+1),IF(B18=Extra!$W$2,VLOOKUP(C18,Extra!$R$4:$AD$8,(O18+5)),IF(B18=Extra!$AA$2,VLOOKUP(C18,Extra!$R$4:$AD$8,(O18+9)),0))))</f>
+      <c r="P19" s="5">
+        <f>IF(B19=0," ",IF(B19=Extra!$S$2,VLOOKUP(C19,Extra!$R$4:$AD$8,O19+1),IF(B19=Extra!$W$2,VLOOKUP(C19,Extra!$R$4:$AD$8,(O19+5)),IF(B19=Extra!$AA$2,VLOOKUP(C19,Extra!$R$4:$AD$8,(O19+9)),0))))</f>
         <v>3</v>
       </c>
-      <c r="Q18" s="5">
-        <f>IF(I18=0," ",IF(I18=Extra!$S$10,VLOOKUP(F18,Extra!$R$12:$X$17,L18+1),IF(I18=Extra!$V$10,VLOOKUP(F18,Extra!$R$12:$X$17,(L18+4)),0)))</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.45">
-      <c r="A19" s="106">
+      <c r="Q19" s="5">
+        <f>IF(I19=0," ",IF(I19=Extra!$S$10,VLOOKUP(F19,Extra!$R$12:$X$17,L19+1),IF(I19=Extra!$V$10,VLOOKUP(F19,Extra!$R$12:$X$17,(L19+4)),0)))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:31" x14ac:dyDescent="0.45">
+      <c r="A20" s="106">
         <f>Angles!A20</f>
         <v>18</v>
       </c>
-      <c r="B19" s="2">
-        <f>IF(A19=0,0,IF(Scores!B20+Scores!C20+Scores!D20=1,1,IF(Scores!B20+Scores!C20+Scores!D20=2,2,IF(Scores!B20+Scores!C20+Scores!D20&gt;=3,3,0))))</f>
-        <v>1</v>
-      </c>
-      <c r="C19" s="2">
+      <c r="B20" s="2">
+        <f>IF(A20=0,0,IF(Scores!B20+Scores!C20+Scores!D20=1,1,IF(Scores!B20+Scores!C20+Scores!D20=2,2,IF(Scores!B20+Scores!C20+Scores!D20&gt;=3,3,0))))</f>
+        <v>1</v>
+      </c>
+      <c r="C20" s="2">
         <f>Scores!E20+Scores!F20+Scores!G20</f>
         <v>1</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D20" s="2">
         <f>Scores!H20+Scores!I20</f>
         <v>1</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E20" s="2">
         <f>Scores!J20+Scores!K20</f>
         <v>2</v>
       </c>
-      <c r="F19" s="2">
-        <f>IF(D19&gt;E19,D19,E19)</f>
-        <v>2</v>
-      </c>
-      <c r="G19" s="2">
+      <c r="F20" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G20" s="2">
         <f>Scores!L20</f>
         <v>1</v>
       </c>
-      <c r="H19" s="2">
+      <c r="H20" s="2">
         <f>Scores!N20</f>
         <v>1</v>
       </c>
-      <c r="I19" s="2">
-        <f>IF(A19=0,0,IF(G19&gt;H19,G19,H19))</f>
-        <v>1</v>
-      </c>
-      <c r="J19" s="2">
+      <c r="I20" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J20" s="2">
         <f>Scores!P20+MAX(Scores!Q20,Scores!M20)</f>
         <v>2</v>
       </c>
-      <c r="K19" s="2">
+      <c r="K20" s="2">
         <f>Scores!R20+MAX(Scores!S20,Scores!O20)</f>
         <v>1</v>
       </c>
-      <c r="L19" s="2">
-        <f>IF(J19&gt;K19,J19,K19)</f>
-        <v>2</v>
-      </c>
-      <c r="M19" s="2">
+      <c r="L20" s="2">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="M20" s="2">
         <f>Scores!T20+Scores!V20</f>
         <v>2</v>
       </c>
-      <c r="N19" s="2">
+      <c r="N20" s="2">
         <f>Scores!U20+Scores!V20</f>
         <v>4</v>
       </c>
-      <c r="O19" s="2">
-        <f>IF(M19&gt;N19,M19,N19)</f>
-        <v>4</v>
-      </c>
-      <c r="P19" s="5">
-        <f>IF(B19=0," ",IF(B19=Extra!$S$2,VLOOKUP(C19,Extra!$R$4:$AD$8,O19+1),IF(B19=Extra!$W$2,VLOOKUP(C19,Extra!$R$4:$AD$8,(O19+5)),IF(B19=Extra!$AA$2,VLOOKUP(C19,Extra!$R$4:$AD$8,(O19+9)),0))))</f>
-        <v>4</v>
-      </c>
-      <c r="Q19" s="5">
-        <f>IF(I19=0," ",IF(I19=Extra!$S$10,VLOOKUP(F19,Extra!$R$12:$X$17,L19+1),IF(I19=Extra!$V$10,VLOOKUP(F19,Extra!$R$12:$X$17,(L19+4)),0)))</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.45">
-      <c r="A20" s="106">
-        <f>Angles!A21</f>
-        <v>19</v>
-      </c>
-      <c r="B20" s="2">
-        <f>IF(A20=0,0,IF(Scores!B21+Scores!C21+Scores!D21=1,1,IF(Scores!B21+Scores!C21+Scores!D21=2,2,IF(Scores!B21+Scores!C21+Scores!D21&gt;=3,3,0))))</f>
-        <v>1</v>
-      </c>
-      <c r="C20" s="2">
-        <f>Scores!E21+Scores!F21+Scores!G21</f>
-        <v>1</v>
-      </c>
-      <c r="D20" s="2">
-        <f>Scores!H21+Scores!I21</f>
-        <v>1</v>
-      </c>
-      <c r="E20" s="2">
-        <f>Scores!J21+Scores!K21</f>
-        <v>2</v>
-      </c>
-      <c r="F20" s="2">
-        <f>IF(D20&gt;E20,D20,E20)</f>
-        <v>2</v>
-      </c>
-      <c r="G20" s="2">
-        <f>Scores!L21</f>
-        <v>1</v>
-      </c>
-      <c r="H20" s="2">
-        <f>Scores!N21</f>
-        <v>1</v>
-      </c>
-      <c r="I20" s="2">
-        <f>IF(A20=0,0,IF(G20&gt;H20,G20,H20))</f>
-        <v>1</v>
-      </c>
-      <c r="J20" s="2">
-        <f>Scores!P21+MAX(Scores!Q21,Scores!M21)</f>
-        <v>1</v>
-      </c>
-      <c r="K20" s="2">
-        <f>Scores!R21+MAX(Scores!S21,Scores!O21)</f>
-        <v>2</v>
-      </c>
-      <c r="L20" s="2">
-        <f>IF(J20&gt;K20,J20,K20)</f>
-        <v>2</v>
-      </c>
-      <c r="M20" s="2">
-        <f>Scores!T21+Scores!V21</f>
-        <v>2</v>
-      </c>
-      <c r="N20" s="2">
-        <f>Scores!U21+Scores!V21</f>
-        <v>4</v>
-      </c>
       <c r="O20" s="2">
-        <f>IF(M20&gt;N20,M20,N20)</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="P20" s="5">
@@ -28570,63 +28536,63 @@
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A21" s="106">
-        <f>Angles!A22</f>
-        <v>20</v>
+        <f>Angles!A21</f>
+        <v>19</v>
       </c>
       <c r="B21" s="2">
-        <f>IF(A21=0,0,IF(Scores!B22+Scores!C22+Scores!D22=1,1,IF(Scores!B22+Scores!C22+Scores!D22=2,2,IF(Scores!B22+Scores!C22+Scores!D22&gt;=3,3,0))))</f>
+        <f>IF(A21=0,0,IF(Scores!B21+Scores!C21+Scores!D21=1,1,IF(Scores!B21+Scores!C21+Scores!D21=2,2,IF(Scores!B21+Scores!C21+Scores!D21&gt;=3,3,0))))</f>
         <v>1</v>
       </c>
       <c r="C21" s="2">
-        <f>Scores!E22+Scores!F22+Scores!G22</f>
+        <f>Scores!E21+Scores!F21+Scores!G21</f>
         <v>1</v>
       </c>
       <c r="D21" s="2">
-        <f>Scores!H22+Scores!I22</f>
+        <f>Scores!H21+Scores!I21</f>
         <v>1</v>
       </c>
       <c r="E21" s="2">
-        <f>Scores!J22+Scores!K22</f>
+        <f>Scores!J21+Scores!K21</f>
         <v>2</v>
       </c>
       <c r="F21" s="2">
-        <f>IF(D21&gt;E21,D21,E21)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="G21" s="2">
-        <f>Scores!L22</f>
+        <f>Scores!L21</f>
         <v>1</v>
       </c>
       <c r="H21" s="2">
-        <f>Scores!N22</f>
+        <f>Scores!N21</f>
         <v>1</v>
       </c>
       <c r="I21" s="2">
-        <f>IF(A21=0,0,IF(G21&gt;H21,G21,H21))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J21" s="2">
-        <f>Scores!P22+MAX(Scores!Q22,Scores!M22)</f>
+        <f>Scores!P21+MAX(Scores!Q21,Scores!M21)</f>
         <v>1</v>
       </c>
       <c r="K21" s="2">
-        <f>Scores!R22+MAX(Scores!S22,Scores!O22)</f>
+        <f>Scores!R21+MAX(Scores!S21,Scores!O21)</f>
         <v>2</v>
       </c>
       <c r="L21" s="2">
-        <f>IF(J21&gt;K21,J21,K21)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="M21" s="2">
-        <f>Scores!T22+Scores!V22</f>
+        <f>Scores!T21+Scores!V21</f>
         <v>2</v>
       </c>
       <c r="N21" s="2">
-        <f>Scores!U22+Scores!V22</f>
+        <f>Scores!U21+Scores!V21</f>
         <v>4</v>
       </c>
       <c r="O21" s="2">
-        <f>IF(M21&gt;N21,M21,N21)</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="P21" s="5">
@@ -28640,63 +28606,63 @@
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A22" s="106">
-        <f>Angles!A23</f>
-        <v>21</v>
+        <f>Angles!A22</f>
+        <v>20</v>
       </c>
       <c r="B22" s="2">
-        <f>IF(A22=0,0,IF(Scores!B23+Scores!C23+Scores!D23=1,1,IF(Scores!B23+Scores!C23+Scores!D23=2,2,IF(Scores!B23+Scores!C23+Scores!D23&gt;=3,3,0))))</f>
+        <f>IF(A22=0,0,IF(Scores!B22+Scores!C22+Scores!D22=1,1,IF(Scores!B22+Scores!C22+Scores!D22=2,2,IF(Scores!B22+Scores!C22+Scores!D22&gt;=3,3,0))))</f>
         <v>1</v>
       </c>
       <c r="C22" s="2">
-        <f>Scores!E23+Scores!F23+Scores!G23</f>
+        <f>Scores!E22+Scores!F22+Scores!G22</f>
         <v>1</v>
       </c>
       <c r="D22" s="2">
-        <f>Scores!H23+Scores!I23</f>
+        <f>Scores!H22+Scores!I22</f>
         <v>1</v>
       </c>
       <c r="E22" s="2">
-        <f>Scores!J23+Scores!K23</f>
+        <f>Scores!J22+Scores!K22</f>
         <v>2</v>
       </c>
       <c r="F22" s="2">
-        <f>IF(D22&gt;E22,D22,E22)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="G22" s="2">
-        <f>Scores!L23</f>
+        <f>Scores!L22</f>
         <v>1</v>
       </c>
       <c r="H22" s="2">
-        <f>Scores!N23</f>
+        <f>Scores!N22</f>
         <v>1</v>
       </c>
       <c r="I22" s="2">
-        <f>IF(A22=0,0,IF(G22&gt;H22,G22,H22))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J22" s="2">
-        <f>Scores!P23+MAX(Scores!Q23,Scores!M23)</f>
+        <f>Scores!P22+MAX(Scores!Q22,Scores!M22)</f>
         <v>1</v>
       </c>
       <c r="K22" s="2">
-        <f>Scores!R23+MAX(Scores!S23,Scores!O23)</f>
+        <f>Scores!R22+MAX(Scores!S22,Scores!O22)</f>
         <v>2</v>
       </c>
       <c r="L22" s="2">
-        <f>IF(J22&gt;K22,J22,K22)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="M22" s="2">
-        <f>Scores!T23+Scores!V23</f>
+        <f>Scores!T22+Scores!V22</f>
         <v>2</v>
       </c>
       <c r="N22" s="2">
-        <f>Scores!U23+Scores!V23</f>
+        <f>Scores!U22+Scores!V22</f>
         <v>4</v>
       </c>
       <c r="O22" s="2">
-        <f>IF(M22&gt;N22,M22,N22)</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="P22" s="5">
@@ -28710,63 +28676,63 @@
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A23" s="106">
-        <f>Angles!A24</f>
-        <v>22</v>
+        <f>Angles!A23</f>
+        <v>21</v>
       </c>
       <c r="B23" s="2">
-        <f>IF(A23=0,0,IF(Scores!B24+Scores!C24+Scores!D24=1,1,IF(Scores!B24+Scores!C24+Scores!D24=2,2,IF(Scores!B24+Scores!C24+Scores!D24&gt;=3,3,0))))</f>
+        <f>IF(A23=0,0,IF(Scores!B23+Scores!C23+Scores!D23=1,1,IF(Scores!B23+Scores!C23+Scores!D23=2,2,IF(Scores!B23+Scores!C23+Scores!D23&gt;=3,3,0))))</f>
         <v>1</v>
       </c>
       <c r="C23" s="2">
-        <f>Scores!E24+Scores!F24+Scores!G24</f>
+        <f>Scores!E23+Scores!F23+Scores!G23</f>
         <v>1</v>
       </c>
       <c r="D23" s="2">
-        <f>Scores!H24+Scores!I24</f>
+        <f>Scores!H23+Scores!I23</f>
         <v>1</v>
       </c>
       <c r="E23" s="2">
-        <f>Scores!J24+Scores!K24</f>
+        <f>Scores!J23+Scores!K23</f>
         <v>2</v>
       </c>
       <c r="F23" s="2">
-        <f>IF(D23&gt;E23,D23,E23)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="G23" s="2">
-        <f>Scores!L24</f>
+        <f>Scores!L23</f>
         <v>1</v>
       </c>
       <c r="H23" s="2">
-        <f>Scores!N24</f>
+        <f>Scores!N23</f>
         <v>1</v>
       </c>
       <c r="I23" s="2">
-        <f>IF(A23=0,0,IF(G23&gt;H23,G23,H23))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J23" s="2">
-        <f>Scores!P24+MAX(Scores!Q24,Scores!M24)</f>
+        <f>Scores!P23+MAX(Scores!Q23,Scores!M23)</f>
         <v>1</v>
       </c>
       <c r="K23" s="2">
-        <f>Scores!R24+MAX(Scores!S24,Scores!O24)</f>
+        <f>Scores!R23+MAX(Scores!S23,Scores!O23)</f>
         <v>2</v>
       </c>
       <c r="L23" s="2">
-        <f>IF(J23&gt;K23,J23,K23)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="M23" s="2">
-        <f>Scores!T24+Scores!V24</f>
+        <f>Scores!T23+Scores!V23</f>
         <v>2</v>
       </c>
       <c r="N23" s="2">
-        <f>Scores!U24+Scores!V24</f>
+        <f>Scores!U23+Scores!V23</f>
         <v>4</v>
       </c>
       <c r="O23" s="2">
-        <f>IF(M23&gt;N23,M23,N23)</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="P23" s="5">
@@ -28780,133 +28746,133 @@
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A24" s="106">
+        <f>Angles!A24</f>
+        <v>22</v>
+      </c>
+      <c r="B24" s="2">
+        <f>IF(A24=0,0,IF(Scores!B24+Scores!C24+Scores!D24=1,1,IF(Scores!B24+Scores!C24+Scores!D24=2,2,IF(Scores!B24+Scores!C24+Scores!D24&gt;=3,3,0))))</f>
+        <v>1</v>
+      </c>
+      <c r="C24" s="2">
+        <f>Scores!E24+Scores!F24+Scores!G24</f>
+        <v>1</v>
+      </c>
+      <c r="D24" s="2">
+        <f>Scores!H24+Scores!I24</f>
+        <v>1</v>
+      </c>
+      <c r="E24" s="2">
+        <f>Scores!J24+Scores!K24</f>
+        <v>2</v>
+      </c>
+      <c r="F24" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G24" s="2">
+        <f>Scores!L24</f>
+        <v>1</v>
+      </c>
+      <c r="H24" s="2">
+        <f>Scores!N24</f>
+        <v>1</v>
+      </c>
+      <c r="I24" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J24" s="2">
+        <f>Scores!P24+MAX(Scores!Q24,Scores!M24)</f>
+        <v>1</v>
+      </c>
+      <c r="K24" s="2">
+        <f>Scores!R24+MAX(Scores!S24,Scores!O24)</f>
+        <v>2</v>
+      </c>
+      <c r="L24" s="2">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="M24" s="2">
+        <f>Scores!T24+Scores!V24</f>
+        <v>2</v>
+      </c>
+      <c r="N24" s="2">
+        <f>Scores!U24+Scores!V24</f>
+        <v>4</v>
+      </c>
+      <c r="O24" s="2">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="P24" s="5">
+        <f>IF(B24=0," ",IF(B24=Extra!$S$2,VLOOKUP(C24,Extra!$R$4:$AD$8,O24+1),IF(B24=Extra!$W$2,VLOOKUP(C24,Extra!$R$4:$AD$8,(O24+5)),IF(B24=Extra!$AA$2,VLOOKUP(C24,Extra!$R$4:$AD$8,(O24+9)),0))))</f>
+        <v>4</v>
+      </c>
+      <c r="Q24" s="5">
+        <f>IF(I24=0," ",IF(I24=Extra!$S$10,VLOOKUP(F24,Extra!$R$12:$X$17,L24+1),IF(I24=Extra!$V$10,VLOOKUP(F24,Extra!$R$12:$X$17,(L24+4)),0)))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:31" x14ac:dyDescent="0.45">
+      <c r="A25" s="106">
         <f>Angles!A25</f>
         <v>23</v>
       </c>
-      <c r="B24" s="2">
-        <f>IF(A24=0,0,IF(Scores!B25+Scores!C25+Scores!D25=1,1,IF(Scores!B25+Scores!C25+Scores!D25=2,2,IF(Scores!B25+Scores!C25+Scores!D25&gt;=3,3,0))))</f>
-        <v>2</v>
-      </c>
-      <c r="C24" s="2">
+      <c r="B25" s="2">
+        <f>IF(A25=0,0,IF(Scores!B25+Scores!C25+Scores!D25=1,1,IF(Scores!B25+Scores!C25+Scores!D25=2,2,IF(Scores!B25+Scores!C25+Scores!D25&gt;=3,3,0))))</f>
+        <v>2</v>
+      </c>
+      <c r="C25" s="2">
         <f>Scores!E25+Scores!F25+Scores!G25</f>
         <v>2</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D25" s="2">
         <f>Scores!H25+Scores!I25</f>
         <v>1</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E25" s="2">
         <f>Scores!J25+Scores!K25</f>
         <v>2</v>
       </c>
-      <c r="F24" s="2">
-        <f>IF(D24&gt;E24,D24,E24)</f>
-        <v>2</v>
-      </c>
-      <c r="G24" s="2">
+      <c r="F25" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G25" s="2">
         <f>Scores!L25</f>
         <v>1</v>
       </c>
-      <c r="H24" s="2">
+      <c r="H25" s="2">
         <f>Scores!N25</f>
         <v>1</v>
       </c>
-      <c r="I24" s="2">
-        <f>IF(A24=0,0,IF(G24&gt;H24,G24,H24))</f>
-        <v>1</v>
-      </c>
-      <c r="J24" s="2">
+      <c r="I25" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J25" s="2">
         <f>Scores!P25+MAX(Scores!Q25,Scores!M25)</f>
         <v>1</v>
       </c>
-      <c r="K24" s="2">
+      <c r="K25" s="2">
         <f>Scores!R25+MAX(Scores!S25,Scores!O25)</f>
         <v>2</v>
       </c>
-      <c r="L24" s="2">
-        <f>IF(J24&gt;K24,J24,K24)</f>
-        <v>2</v>
-      </c>
-      <c r="M24" s="2">
+      <c r="L25" s="2">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="M25" s="2">
         <f>Scores!T25+Scores!V25</f>
         <v>3</v>
       </c>
-      <c r="N24" s="2">
+      <c r="N25" s="2">
         <f>Scores!U25+Scores!V25</f>
         <v>4</v>
       </c>
-      <c r="O24" s="2">
-        <f>IF(M24&gt;N24,M24,N24)</f>
-        <v>4</v>
-      </c>
-      <c r="P24" s="5">
-        <f>IF(B24=0," ",IF(B24=Extra!$S$2,VLOOKUP(C24,Extra!$R$4:$AD$8,O24+1),IF(B24=Extra!$W$2,VLOOKUP(C24,Extra!$R$4:$AD$8,(O24+5)),IF(B24=Extra!$AA$2,VLOOKUP(C24,Extra!$R$4:$AD$8,(O24+9)),0))))</f>
-        <v>6</v>
-      </c>
-      <c r="Q24" s="5">
-        <f>IF(I24=0," ",IF(I24=Extra!$S$10,VLOOKUP(F24,Extra!$R$12:$X$17,L24+1),IF(I24=Extra!$V$10,VLOOKUP(F24,Extra!$R$12:$X$17,(L24+4)),0)))</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.45">
-      <c r="A25" s="106">
-        <f>Angles!A26</f>
-        <v>24</v>
-      </c>
-      <c r="B25" s="2">
-        <f>IF(A25=0,0,IF(Scores!B26+Scores!C26+Scores!D26=1,1,IF(Scores!B26+Scores!C26+Scores!D26=2,2,IF(Scores!B26+Scores!C26+Scores!D26&gt;=3,3,0))))</f>
-        <v>2</v>
-      </c>
-      <c r="C25" s="2">
-        <f>Scores!E26+Scores!F26+Scores!G26</f>
-        <v>2</v>
-      </c>
-      <c r="D25" s="2">
-        <f>Scores!H26+Scores!I26</f>
-        <v>1</v>
-      </c>
-      <c r="E25" s="2">
-        <f>Scores!J26+Scores!K26</f>
-        <v>2</v>
-      </c>
-      <c r="F25" s="2">
-        <f>IF(D25&gt;E25,D25,E25)</f>
-        <v>2</v>
-      </c>
-      <c r="G25" s="2">
-        <f>Scores!L26</f>
-        <v>1</v>
-      </c>
-      <c r="H25" s="2">
-        <f>Scores!N26</f>
-        <v>1</v>
-      </c>
-      <c r="I25" s="2">
-        <f>IF(A25=0,0,IF(G25&gt;H25,G25,H25))</f>
-        <v>1</v>
-      </c>
-      <c r="J25" s="2">
-        <f>Scores!P26+MAX(Scores!Q26,Scores!M26)</f>
-        <v>1</v>
-      </c>
-      <c r="K25" s="2">
-        <f>Scores!R26+MAX(Scores!S26,Scores!O26)</f>
-        <v>2</v>
-      </c>
-      <c r="L25" s="2">
-        <f>IF(J25&gt;K25,J25,K25)</f>
-        <v>2</v>
-      </c>
-      <c r="M25" s="2">
-        <f>Scores!T26+Scores!V26</f>
-        <v>3</v>
-      </c>
-      <c r="N25" s="2">
-        <f>Scores!U26+Scores!V26</f>
-        <v>4</v>
-      </c>
       <c r="O25" s="2">
-        <f>IF(M25&gt;N25,M25,N25)</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="P25" s="5">
@@ -28920,63 +28886,63 @@
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A26" s="106">
-        <f>Angles!A27</f>
-        <v>25</v>
+        <f>Angles!A26</f>
+        <v>24</v>
       </c>
       <c r="B26" s="2">
-        <f>IF(A26=0,0,IF(Scores!B27+Scores!C27+Scores!D27=1,1,IF(Scores!B27+Scores!C27+Scores!D27=2,2,IF(Scores!B27+Scores!C27+Scores!D27&gt;=3,3,0))))</f>
+        <f>IF(A26=0,0,IF(Scores!B26+Scores!C26+Scores!D26=1,1,IF(Scores!B26+Scores!C26+Scores!D26=2,2,IF(Scores!B26+Scores!C26+Scores!D26&gt;=3,3,0))))</f>
         <v>2</v>
       </c>
       <c r="C26" s="2">
-        <f>Scores!E27+Scores!F27+Scores!G27</f>
+        <f>Scores!E26+Scores!F26+Scores!G26</f>
         <v>2</v>
       </c>
       <c r="D26" s="2">
-        <f>Scores!H27+Scores!I27</f>
+        <f>Scores!H26+Scores!I26</f>
         <v>1</v>
       </c>
       <c r="E26" s="2">
-        <f>Scores!J27+Scores!K27</f>
+        <f>Scores!J26+Scores!K26</f>
         <v>2</v>
       </c>
       <c r="F26" s="2">
-        <f>IF(D26&gt;E26,D26,E26)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="G26" s="2">
-        <f>Scores!L27</f>
+        <f>Scores!L26</f>
         <v>1</v>
       </c>
       <c r="H26" s="2">
-        <f>Scores!N27</f>
+        <f>Scores!N26</f>
         <v>1</v>
       </c>
       <c r="I26" s="2">
-        <f>IF(A26=0,0,IF(G26&gt;H26,G26,H26))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J26" s="2">
-        <f>Scores!P27+MAX(Scores!Q27,Scores!M27)</f>
+        <f>Scores!P26+MAX(Scores!Q26,Scores!M26)</f>
         <v>1</v>
       </c>
       <c r="K26" s="2">
-        <f>Scores!R27+MAX(Scores!S27,Scores!O27)</f>
+        <f>Scores!R26+MAX(Scores!S26,Scores!O26)</f>
         <v>2</v>
       </c>
       <c r="L26" s="2">
-        <f>IF(J26&gt;K26,J26,K26)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="M26" s="2">
-        <f>Scores!T27+Scores!V27</f>
+        <f>Scores!T26+Scores!V26</f>
         <v>3</v>
       </c>
       <c r="N26" s="2">
-        <f>Scores!U27+Scores!V27</f>
+        <f>Scores!U26+Scores!V26</f>
         <v>4</v>
       </c>
       <c r="O26" s="2">
-        <f>IF(M26&gt;N26,M26,N26)</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="P26" s="5">
@@ -28990,63 +28956,63 @@
     </row>
     <row r="27" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A27" s="106">
-        <f>Angles!A28</f>
-        <v>26</v>
+        <f>Angles!A27</f>
+        <v>25</v>
       </c>
       <c r="B27" s="2">
-        <f>IF(A27=0,0,IF(Scores!B28+Scores!C28+Scores!D28=1,1,IF(Scores!B28+Scores!C28+Scores!D28=2,2,IF(Scores!B28+Scores!C28+Scores!D28&gt;=3,3,0))))</f>
+        <f>IF(A27=0,0,IF(Scores!B27+Scores!C27+Scores!D27=1,1,IF(Scores!B27+Scores!C27+Scores!D27=2,2,IF(Scores!B27+Scores!C27+Scores!D27&gt;=3,3,0))))</f>
         <v>2</v>
       </c>
       <c r="C27" s="2">
-        <f>Scores!E28+Scores!F28+Scores!G28</f>
+        <f>Scores!E27+Scores!F27+Scores!G27</f>
         <v>2</v>
       </c>
       <c r="D27" s="2">
-        <f>Scores!H28+Scores!I28</f>
-        <v>2</v>
+        <f>Scores!H27+Scores!I27</f>
+        <v>1</v>
       </c>
       <c r="E27" s="2">
-        <f>Scores!J28+Scores!K28</f>
+        <f>Scores!J27+Scores!K27</f>
         <v>2</v>
       </c>
       <c r="F27" s="2">
-        <f>IF(D27&gt;E27,D27,E27)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="G27" s="2">
-        <f>Scores!L28</f>
+        <f>Scores!L27</f>
         <v>1</v>
       </c>
       <c r="H27" s="2">
-        <f>Scores!N28</f>
+        <f>Scores!N27</f>
         <v>1</v>
       </c>
       <c r="I27" s="2">
-        <f>IF(A27=0,0,IF(G27&gt;H27,G27,H27))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J27" s="2">
-        <f>Scores!P28+MAX(Scores!Q28,Scores!M28)</f>
-        <v>2</v>
+        <f>Scores!P27+MAX(Scores!Q27,Scores!M27)</f>
+        <v>1</v>
       </c>
       <c r="K27" s="2">
-        <f>Scores!R28+MAX(Scores!S28,Scores!O28)</f>
+        <f>Scores!R27+MAX(Scores!S27,Scores!O27)</f>
         <v>2</v>
       </c>
       <c r="L27" s="2">
-        <f>IF(J27&gt;K27,J27,K27)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="M27" s="2">
-        <f>Scores!T28+Scores!V28</f>
+        <f>Scores!T27+Scores!V27</f>
         <v>3</v>
       </c>
       <c r="N27" s="2">
-        <f>Scores!U28+Scores!V28</f>
+        <f>Scores!U27+Scores!V27</f>
         <v>4</v>
       </c>
       <c r="O27" s="2">
-        <f>IF(M27&gt;N27,M27,N27)</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="P27" s="5">
@@ -29059,36 +29025,74 @@
       </c>
     </row>
     <row r="28" spans="1:31" x14ac:dyDescent="0.45">
-      <c r="A28"/>
-      <c r="B28"/>
-      <c r="C28"/>
-      <c r="D28"/>
-      <c r="E28"/>
-      <c r="F28"/>
-      <c r="G28"/>
-      <c r="H28"/>
-      <c r="I28"/>
-      <c r="J28"/>
-      <c r="K28"/>
-      <c r="L28"/>
-      <c r="M28"/>
-      <c r="N28"/>
-      <c r="O28"/>
-      <c r="P28"/>
-      <c r="Q28"/>
-      <c r="S28"/>
-      <c r="T28"/>
-      <c r="U28"/>
-      <c r="V28"/>
-      <c r="W28"/>
-      <c r="X28"/>
-      <c r="Y28"/>
-      <c r="Z28"/>
-      <c r="AA28"/>
-      <c r="AB28"/>
-      <c r="AC28"/>
-      <c r="AD28"/>
-      <c r="AE28"/>
+      <c r="A28" s="106">
+        <f>Angles!A28</f>
+        <v>26</v>
+      </c>
+      <c r="B28" s="2">
+        <f>IF(A28=0,0,IF(Scores!B28+Scores!C28+Scores!D28=1,1,IF(Scores!B28+Scores!C28+Scores!D28=2,2,IF(Scores!B28+Scores!C28+Scores!D28&gt;=3,3,0))))</f>
+        <v>2</v>
+      </c>
+      <c r="C28" s="2">
+        <f>Scores!E28+Scores!F28+Scores!G28</f>
+        <v>2</v>
+      </c>
+      <c r="D28" s="2">
+        <f>Scores!H28+Scores!I28</f>
+        <v>2</v>
+      </c>
+      <c r="E28" s="2">
+        <f>Scores!J28+Scores!K28</f>
+        <v>2</v>
+      </c>
+      <c r="F28" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G28" s="2">
+        <f>Scores!L28</f>
+        <v>1</v>
+      </c>
+      <c r="H28" s="2">
+        <f>Scores!N28</f>
+        <v>1</v>
+      </c>
+      <c r="I28" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J28" s="2">
+        <f>Scores!P28+MAX(Scores!Q28,Scores!M28)</f>
+        <v>2</v>
+      </c>
+      <c r="K28" s="2">
+        <f>Scores!R28+MAX(Scores!S28,Scores!O28)</f>
+        <v>2</v>
+      </c>
+      <c r="L28" s="2">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="M28" s="2">
+        <f>Scores!T28+Scores!V28</f>
+        <v>3</v>
+      </c>
+      <c r="N28" s="2">
+        <f>Scores!U28+Scores!V28</f>
+        <v>4</v>
+      </c>
+      <c r="O28" s="2">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="P28" s="5">
+        <f>IF(B28=0," ",IF(B28=Extra!$S$2,VLOOKUP(C28,Extra!$R$4:$AD$8,O28+1),IF(B28=Extra!$W$2,VLOOKUP(C28,Extra!$R$4:$AD$8,(O28+5)),IF(B28=Extra!$AA$2,VLOOKUP(C28,Extra!$R$4:$AD$8,(O28+9)),0))))</f>
+        <v>6</v>
+      </c>
+      <c r="Q28" s="5">
+        <f>IF(I28=0," ",IF(I28=Extra!$S$10,VLOOKUP(F28,Extra!$R$12:$X$17,L28+1),IF(I28=Extra!$V$10,VLOOKUP(F28,Extra!$R$12:$X$17,(L28+4)),0)))</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="29" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A29"/>
@@ -29239,6 +29243,7 @@
     <row r="51" customFormat="1" x14ac:dyDescent="0.45"/>
     <row r="52" customFormat="1" x14ac:dyDescent="0.45"/>
     <row r="53" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="54" customFormat="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -29250,7 +29255,7 @@
   <dimension ref="A1:AH32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -29318,7 +29323,7 @@
     </row>
     <row r="2" spans="1:34" ht="20.65" x14ac:dyDescent="0.6">
       <c r="A2" s="119">
-        <f>AVERAGE(Reba!P2:P998)</f>
+        <f>AVERAGE(Reba!P3:P999)</f>
         <v>4.7307692307692308</v>
       </c>
       <c r="B2" s="108"/>
@@ -29331,7 +29336,7 @@
       </c>
       <c r="E2" s="108"/>
       <c r="F2" s="119">
-        <f>AVERAGE(Reba!Q2:Q998)</f>
+        <f>AVERAGE(Reba!Q3:Q999)</f>
         <v>2.5769230769230771</v>
       </c>
       <c r="G2" s="108"/>
@@ -30881,8 +30886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC21BA3E-0D99-4DBD-ACE1-ABFCA6A967C0}">
   <dimension ref="A1:AP48"/>
   <sheetViews>
-    <sheetView zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="AF27" sqref="AF27"/>
+    <sheetView topLeftCell="A14" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+      <selection activeCell="H48" sqref="H48:M48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -30930,24 +30935,24 @@
       <c r="C2" s="14"/>
       <c r="D2" s="15"/>
       <c r="E2" s="16"/>
-      <c r="F2" s="159" t="s">
+      <c r="F2" s="123" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="176" t="s">
+      <c r="G2" s="126" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="176"/>
-      <c r="I2" s="176"/>
-      <c r="J2" s="176"/>
-      <c r="K2" s="176"/>
-      <c r="L2" s="176"/>
-      <c r="M2" s="176"/>
-      <c r="N2" s="176"/>
-      <c r="O2" s="176"/>
-      <c r="P2" s="176"/>
-      <c r="Q2" s="176"/>
-      <c r="R2" s="176"/>
-      <c r="S2" s="176"/>
+      <c r="H2" s="126"/>
+      <c r="I2" s="126"/>
+      <c r="J2" s="126"/>
+      <c r="K2" s="126"/>
+      <c r="L2" s="126"/>
+      <c r="M2" s="126"/>
+      <c r="N2" s="126"/>
+      <c r="O2" s="126"/>
+      <c r="P2" s="126"/>
+      <c r="Q2" s="126"/>
+      <c r="R2" s="126"/>
+      <c r="S2" s="126"/>
       <c r="T2" s="14"/>
       <c r="U2" s="19" t="s">
         <v>9</v>
@@ -30967,26 +30972,26 @@
       <c r="C3" s="14"/>
       <c r="D3" s="15"/>
       <c r="E3" s="16"/>
-      <c r="F3" s="159"/>
+      <c r="F3" s="123"/>
       <c r="G3" s="18"/>
-      <c r="H3" s="176">
-        <v>1</v>
-      </c>
-      <c r="I3" s="176"/>
-      <c r="J3" s="176"/>
-      <c r="K3" s="176"/>
-      <c r="L3" s="176">
-        <v>2</v>
-      </c>
-      <c r="M3" s="176"/>
-      <c r="N3" s="176"/>
-      <c r="O3" s="176"/>
-      <c r="P3" s="176">
+      <c r="H3" s="126">
+        <v>1</v>
+      </c>
+      <c r="I3" s="126"/>
+      <c r="J3" s="126"/>
+      <c r="K3" s="126"/>
+      <c r="L3" s="126">
+        <v>2</v>
+      </c>
+      <c r="M3" s="126"/>
+      <c r="N3" s="126"/>
+      <c r="O3" s="126"/>
+      <c r="P3" s="126">
         <v>3</v>
       </c>
-      <c r="Q3" s="176"/>
-      <c r="R3" s="176"/>
-      <c r="S3" s="176"/>
+      <c r="Q3" s="126"/>
+      <c r="R3" s="126"/>
+      <c r="S3" s="126"/>
       <c r="T3" s="14"/>
       <c r="U3" s="14"/>
       <c r="V3" s="14"/>
@@ -31015,22 +31020,22 @@
       <c r="C4" s="14"/>
       <c r="D4" s="15"/>
       <c r="E4" s="16"/>
-      <c r="F4" s="159"/>
-      <c r="G4" s="177" t="s">
+      <c r="F4" s="123"/>
+      <c r="G4" s="124" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="178"/>
-      <c r="I4" s="178"/>
-      <c r="J4" s="178"/>
-      <c r="K4" s="178"/>
-      <c r="L4" s="178"/>
-      <c r="M4" s="178"/>
-      <c r="N4" s="178"/>
-      <c r="O4" s="178"/>
-      <c r="P4" s="178"/>
-      <c r="Q4" s="178"/>
-      <c r="R4" s="178"/>
-      <c r="S4" s="178"/>
+      <c r="H4" s="125"/>
+      <c r="I4" s="125"/>
+      <c r="J4" s="125"/>
+      <c r="K4" s="125"/>
+      <c r="L4" s="125"/>
+      <c r="M4" s="125"/>
+      <c r="N4" s="125"/>
+      <c r="O4" s="125"/>
+      <c r="P4" s="125"/>
+      <c r="Q4" s="125"/>
+      <c r="R4" s="125"/>
+      <c r="S4" s="125"/>
       <c r="T4" s="14"/>
       <c r="U4" s="14"/>
       <c r="V4" s="14"/>
@@ -31058,8 +31063,8 @@
       <c r="C5" s="14"/>
       <c r="D5" s="15"/>
       <c r="E5" s="14"/>
-      <c r="F5" s="159"/>
-      <c r="G5" s="177"/>
+      <c r="F5" s="123"/>
+      <c r="G5" s="124"/>
       <c r="H5" s="22">
         <v>1</v>
       </c>
@@ -31122,8 +31127,8 @@
       <c r="B6" s="14"/>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
-      <c r="E6" s="170"/>
-      <c r="F6" s="172" t="s">
+      <c r="E6" s="127"/>
+      <c r="F6" s="129" t="s">
         <v>11</v>
       </c>
       <c r="G6" s="23">
@@ -31191,8 +31196,8 @@
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
-      <c r="E7" s="171"/>
-      <c r="F7" s="172"/>
+      <c r="E7" s="128"/>
+      <c r="F7" s="129"/>
       <c r="G7" s="23">
         <v>2</v>
       </c>
@@ -31263,7 +31268,7 @@
       <c r="E8" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="172"/>
+      <c r="F8" s="129"/>
       <c r="G8" s="23">
         <v>3</v>
       </c>
@@ -31332,7 +31337,7 @@
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
       <c r="E9" s="15"/>
-      <c r="F9" s="172"/>
+      <c r="F9" s="129"/>
       <c r="G9" s="23">
         <v>4</v>
       </c>
@@ -31380,7 +31385,7 @@
       <c r="W9" s="14"/>
       <c r="X9" s="14"/>
       <c r="Y9" s="14"/>
-      <c r="Z9" s="173"/>
+      <c r="Z9" s="130"/>
       <c r="AA9" s="20"/>
       <c r="AD9" s="1"/>
       <c r="AE9" s="1"/>
@@ -31403,7 +31408,7 @@
       <c r="C10" s="14"/>
       <c r="D10" s="14"/>
       <c r="E10" s="15"/>
-      <c r="F10" s="172"/>
+      <c r="F10" s="129"/>
       <c r="G10" s="23">
         <v>5</v>
       </c>
@@ -31451,7 +31456,7 @@
       <c r="W10" s="14"/>
       <c r="X10" s="14"/>
       <c r="Y10" s="14"/>
-      <c r="Z10" s="174"/>
+      <c r="Z10" s="131"/>
       <c r="AA10" s="20"/>
       <c r="AC10" s="66"/>
       <c r="AD10" s="66"/>
@@ -31506,18 +31511,18 @@
       <c r="C12" s="14"/>
       <c r="D12" s="15"/>
       <c r="E12" s="27"/>
-      <c r="F12" s="159" t="s">
+      <c r="F12" s="123" t="s">
         <v>21</v>
       </c>
-      <c r="G12" s="175" t="s">
+      <c r="G12" s="132" t="s">
         <v>22</v>
       </c>
-      <c r="H12" s="175"/>
-      <c r="I12" s="175"/>
-      <c r="J12" s="175"/>
-      <c r="K12" s="175"/>
-      <c r="L12" s="175"/>
-      <c r="M12" s="175"/>
+      <c r="H12" s="132"/>
+      <c r="I12" s="132"/>
+      <c r="J12" s="132"/>
+      <c r="K12" s="132"/>
+      <c r="L12" s="132"/>
+      <c r="M12" s="132"/>
       <c r="N12" s="28"/>
       <c r="O12" s="29"/>
       <c r="P12" s="29"/>
@@ -31548,18 +31553,18 @@
       <c r="C13" s="14"/>
       <c r="D13" s="15"/>
       <c r="E13" s="14"/>
-      <c r="F13" s="159"/>
+      <c r="F13" s="123"/>
       <c r="G13" s="31"/>
-      <c r="H13" s="175">
-        <v>1</v>
-      </c>
-      <c r="I13" s="175"/>
-      <c r="J13" s="175"/>
-      <c r="K13" s="175">
-        <v>2</v>
-      </c>
-      <c r="L13" s="175"/>
-      <c r="M13" s="175"/>
+      <c r="H13" s="132">
+        <v>1</v>
+      </c>
+      <c r="I13" s="132"/>
+      <c r="J13" s="132"/>
+      <c r="K13" s="132">
+        <v>2</v>
+      </c>
+      <c r="L13" s="132"/>
+      <c r="M13" s="132"/>
       <c r="N13" s="29"/>
       <c r="O13" s="29"/>
       <c r="P13" s="29"/>
@@ -31588,16 +31593,16 @@
       <c r="C14" s="14"/>
       <c r="D14" s="15"/>
       <c r="E14" s="15"/>
-      <c r="F14" s="159"/>
-      <c r="G14" s="167" t="s">
+      <c r="F14" s="123"/>
+      <c r="G14" s="133" t="s">
         <v>24</v>
       </c>
-      <c r="H14" s="168"/>
-      <c r="I14" s="168"/>
-      <c r="J14" s="168"/>
-      <c r="K14" s="168"/>
-      <c r="L14" s="168"/>
-      <c r="M14" s="168"/>
+      <c r="H14" s="134"/>
+      <c r="I14" s="134"/>
+      <c r="J14" s="134"/>
+      <c r="K14" s="134"/>
+      <c r="L14" s="134"/>
+      <c r="M14" s="134"/>
       <c r="N14" s="29"/>
       <c r="O14" s="29"/>
       <c r="P14" s="29"/>
@@ -31626,8 +31631,8 @@
       <c r="C15" s="14"/>
       <c r="D15" s="15"/>
       <c r="E15" s="14"/>
-      <c r="F15" s="159"/>
-      <c r="G15" s="167"/>
+      <c r="F15" s="123"/>
+      <c r="G15" s="133"/>
       <c r="H15" s="32">
         <v>1</v>
       </c>
@@ -31676,7 +31681,7 @@
       <c r="C16" s="14"/>
       <c r="D16" s="15"/>
       <c r="E16" s="14"/>
-      <c r="F16" s="169" t="s">
+      <c r="F16" s="135" t="s">
         <v>19</v>
       </c>
       <c r="G16" s="33">
@@ -31728,7 +31733,7 @@
       <c r="C17" s="14"/>
       <c r="D17" s="15"/>
       <c r="E17" s="14"/>
-      <c r="F17" s="169"/>
+      <c r="F17" s="135"/>
       <c r="G17" s="33">
         <v>2</v>
       </c>
@@ -31762,7 +31767,7 @@
       <c r="W17" s="14"/>
       <c r="X17" s="14"/>
       <c r="Y17" s="14"/>
-      <c r="Z17" s="165"/>
+      <c r="Z17" s="144"/>
       <c r="AA17" s="20"/>
       <c r="AD17" s="1"/>
       <c r="AE17" s="1"/>
@@ -31779,8 +31784,8 @@
       <c r="B18" s="14"/>
       <c r="C18" s="14"/>
       <c r="D18" s="14"/>
-      <c r="E18" s="156"/>
-      <c r="F18" s="169"/>
+      <c r="E18" s="136"/>
+      <c r="F18" s="135"/>
       <c r="G18" s="33">
         <v>3</v>
       </c>
@@ -31814,7 +31819,7 @@
       <c r="W18" s="14"/>
       <c r="X18" s="14"/>
       <c r="Y18" s="14"/>
-      <c r="Z18" s="166"/>
+      <c r="Z18" s="145"/>
       <c r="AA18" s="20"/>
       <c r="AD18" s="1"/>
       <c r="AE18" s="1"/>
@@ -31831,8 +31836,8 @@
       <c r="B19" s="14"/>
       <c r="C19" s="14"/>
       <c r="D19" s="14"/>
-      <c r="E19" s="157"/>
-      <c r="F19" s="169"/>
+      <c r="E19" s="137"/>
+      <c r="F19" s="135"/>
       <c r="G19" s="33">
         <v>4</v>
       </c>
@@ -31881,7 +31886,7 @@
       <c r="E20" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="F20" s="169"/>
+      <c r="F20" s="135"/>
       <c r="G20" s="33">
         <v>5</v>
       </c>
@@ -31926,7 +31931,7 @@
       <c r="C21" s="14"/>
       <c r="D21" s="15"/>
       <c r="E21" s="14"/>
-      <c r="F21" s="169"/>
+      <c r="F21" s="135"/>
       <c r="G21" s="33">
         <v>6</v>
       </c>
@@ -32028,23 +32033,23 @@
       <c r="C23" s="14"/>
       <c r="D23" s="15"/>
       <c r="E23" s="14"/>
-      <c r="F23" s="158" t="s">
+      <c r="F23" s="138" t="s">
         <v>33</v>
       </c>
-      <c r="G23" s="159" t="s">
+      <c r="G23" s="123" t="s">
         <v>34</v>
       </c>
-      <c r="H23" s="159"/>
-      <c r="I23" s="159"/>
-      <c r="J23" s="159"/>
-      <c r="K23" s="159"/>
-      <c r="L23" s="159"/>
-      <c r="M23" s="159"/>
-      <c r="N23" s="159"/>
-      <c r="O23" s="159"/>
-      <c r="P23" s="159"/>
-      <c r="Q23" s="159"/>
-      <c r="R23" s="159"/>
+      <c r="H23" s="123"/>
+      <c r="I23" s="123"/>
+      <c r="J23" s="123"/>
+      <c r="K23" s="123"/>
+      <c r="L23" s="123"/>
+      <c r="M23" s="123"/>
+      <c r="N23" s="123"/>
+      <c r="O23" s="123"/>
+      <c r="P23" s="123"/>
+      <c r="Q23" s="123"/>
+      <c r="R23" s="123"/>
       <c r="S23" s="26"/>
       <c r="T23" s="14"/>
       <c r="U23" s="14"/>
@@ -32074,21 +32079,21 @@
       <c r="C24" s="14"/>
       <c r="D24" s="15"/>
       <c r="E24" s="14"/>
-      <c r="F24" s="158"/>
-      <c r="G24" s="160" t="s">
+      <c r="F24" s="138"/>
+      <c r="G24" s="139" t="s">
         <v>35</v>
       </c>
-      <c r="H24" s="160"/>
-      <c r="I24" s="160"/>
-      <c r="J24" s="160"/>
-      <c r="K24" s="160"/>
-      <c r="L24" s="160"/>
-      <c r="M24" s="160"/>
-      <c r="N24" s="160"/>
-      <c r="O24" s="160"/>
-      <c r="P24" s="160"/>
-      <c r="Q24" s="160"/>
-      <c r="R24" s="160"/>
+      <c r="H24" s="139"/>
+      <c r="I24" s="139"/>
+      <c r="J24" s="139"/>
+      <c r="K24" s="139"/>
+      <c r="L24" s="139"/>
+      <c r="M24" s="139"/>
+      <c r="N24" s="139"/>
+      <c r="O24" s="139"/>
+      <c r="P24" s="139"/>
+      <c r="Q24" s="139"/>
+      <c r="R24" s="139"/>
       <c r="S24" s="26"/>
       <c r="T24" s="14"/>
       <c r="U24" s="14"/>
@@ -32096,7 +32101,7 @@
       <c r="W24" s="14"/>
       <c r="X24" s="14"/>
       <c r="Y24" s="14"/>
-      <c r="Z24" s="161"/>
+      <c r="Z24" s="140"/>
       <c r="AA24" s="20"/>
       <c r="AC24" s="1"/>
       <c r="AE24" s="1"/>
@@ -32117,20 +32122,20 @@
       <c r="B25" s="14"/>
       <c r="C25" s="14"/>
       <c r="D25" s="14"/>
-      <c r="E25" s="163"/>
-      <c r="F25" s="158"/>
-      <c r="G25" s="160"/>
-      <c r="H25" s="160"/>
-      <c r="I25" s="160"/>
-      <c r="J25" s="160"/>
-      <c r="K25" s="160"/>
-      <c r="L25" s="160"/>
-      <c r="M25" s="160"/>
-      <c r="N25" s="160"/>
-      <c r="O25" s="160"/>
-      <c r="P25" s="160"/>
-      <c r="Q25" s="160"/>
-      <c r="R25" s="160"/>
+      <c r="E25" s="142"/>
+      <c r="F25" s="138"/>
+      <c r="G25" s="139"/>
+      <c r="H25" s="139"/>
+      <c r="I25" s="139"/>
+      <c r="J25" s="139"/>
+      <c r="K25" s="139"/>
+      <c r="L25" s="139"/>
+      <c r="M25" s="139"/>
+      <c r="N25" s="139"/>
+      <c r="O25" s="139"/>
+      <c r="P25" s="139"/>
+      <c r="Q25" s="139"/>
+      <c r="R25" s="139"/>
       <c r="S25" s="26"/>
       <c r="T25" s="14"/>
       <c r="U25" s="14"/>
@@ -32138,7 +32143,7 @@
       <c r="W25" s="14"/>
       <c r="X25" s="14"/>
       <c r="Y25" s="14"/>
-      <c r="Z25" s="162"/>
+      <c r="Z25" s="141"/>
       <c r="AA25" s="20"/>
       <c r="AC25" s="1"/>
       <c r="AE25" s="1"/>
@@ -32159,8 +32164,8 @@
       <c r="B26" s="14"/>
       <c r="C26" s="14"/>
       <c r="D26" s="14"/>
-      <c r="E26" s="164"/>
-      <c r="F26" s="158"/>
+      <c r="E26" s="143"/>
+      <c r="F26" s="138"/>
       <c r="G26" s="34">
         <v>1</v>
       </c>
@@ -32348,7 +32353,7 @@
       <c r="W28" s="14"/>
       <c r="X28" s="14"/>
       <c r="Y28" s="14"/>
-      <c r="Z28" s="131">
+      <c r="Z28" s="154">
         <f>Extra!F2</f>
         <v>2.5769230769230771</v>
       </c>
@@ -32421,7 +32426,7 @@
       <c r="W29" s="14"/>
       <c r="X29" s="14"/>
       <c r="Y29" s="14"/>
-      <c r="Z29" s="132"/>
+      <c r="Z29" s="155"/>
       <c r="AA29" s="20"/>
       <c r="AC29" s="1"/>
       <c r="AE29" s="1"/>
@@ -32444,7 +32449,7 @@
       <c r="B30" s="14"/>
       <c r="C30" s="14"/>
       <c r="D30" s="14"/>
-      <c r="E30" s="133">
+      <c r="E30" s="156">
         <f>Extra!A2</f>
         <v>4.7307692307692308</v>
       </c>
@@ -32521,7 +32526,7 @@
       <c r="B31" s="14"/>
       <c r="C31" s="14"/>
       <c r="D31" s="14"/>
-      <c r="E31" s="134"/>
+      <c r="E31" s="157"/>
       <c r="F31" s="36">
         <v>5</v>
       </c>
@@ -32646,7 +32651,7 @@
       <c r="W32" s="14"/>
       <c r="X32" s="14"/>
       <c r="Y32" s="14"/>
-      <c r="Z32" s="135">
+      <c r="Z32" s="158">
         <f>Extra!H2</f>
         <v>0</v>
       </c>
@@ -32721,7 +32726,7 @@
       <c r="W33" s="14"/>
       <c r="X33" s="14"/>
       <c r="Y33" s="14"/>
-      <c r="Z33" s="136"/>
+      <c r="Z33" s="159"/>
       <c r="AA33" s="20"/>
       <c r="AC33" s="1"/>
       <c r="AE33" s="1"/>
@@ -32744,7 +32749,7 @@
       <c r="B34" s="15"/>
       <c r="C34" s="14"/>
       <c r="D34" s="14"/>
-      <c r="E34" s="135">
+      <c r="E34" s="158">
         <f>Extra!C2</f>
         <v>0</v>
       </c>
@@ -32808,7 +32813,7 @@
       <c r="B35" s="15"/>
       <c r="C35" s="14"/>
       <c r="D35" s="14"/>
-      <c r="E35" s="136"/>
+      <c r="E35" s="159"/>
       <c r="F35" s="36">
         <v>9</v>
       </c>
@@ -33040,7 +33045,7 @@
       <c r="W38" s="14"/>
       <c r="X38" s="14"/>
       <c r="Y38" s="14"/>
-      <c r="Z38" s="137">
+      <c r="Z38" s="160">
         <f>Extra!I2</f>
         <v>2.5769230769230771</v>
       </c>
@@ -33053,7 +33058,7 @@
       <c r="B39" s="14"/>
       <c r="C39" s="15"/>
       <c r="D39" s="14"/>
-      <c r="E39" s="139">
+      <c r="E39" s="162">
         <f>Extra!D2</f>
         <v>4.7307692307692308</v>
       </c>
@@ -33079,7 +33084,7 @@
       <c r="W39" s="14"/>
       <c r="X39" s="14"/>
       <c r="Y39" s="14"/>
-      <c r="Z39" s="138"/>
+      <c r="Z39" s="161"/>
       <c r="AA39" s="20"/>
     </row>
     <row r="40" spans="1:42" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -33089,28 +33094,28 @@
       <c r="B40" s="14"/>
       <c r="C40" s="15"/>
       <c r="D40" s="14"/>
-      <c r="E40" s="140"/>
-      <c r="F40" s="141">
+      <c r="E40" s="163"/>
+      <c r="F40" s="164">
         <f>Extra!K2</f>
         <v>4</v>
       </c>
-      <c r="G40" s="142"/>
-      <c r="H40" s="143"/>
-      <c r="I40" s="147" t="s">
+      <c r="G40" s="165"/>
+      <c r="H40" s="166"/>
+      <c r="I40" s="170" t="s">
         <v>66</v>
       </c>
-      <c r="J40" s="148"/>
-      <c r="K40" s="148"/>
-      <c r="L40" s="149"/>
-      <c r="M40" s="150">
+      <c r="J40" s="171"/>
+      <c r="K40" s="171"/>
+      <c r="L40" s="172"/>
+      <c r="M40" s="173">
         <f>Extra!M2</f>
         <v>0</v>
       </c>
-      <c r="N40" s="151"/>
-      <c r="O40" s="151"/>
-      <c r="P40" s="151"/>
-      <c r="Q40" s="151"/>
-      <c r="R40" s="152"/>
+      <c r="N40" s="174"/>
+      <c r="O40" s="174"/>
+      <c r="P40" s="174"/>
+      <c r="Q40" s="174"/>
+      <c r="R40" s="175"/>
       <c r="S40" s="14"/>
       <c r="T40" s="14"/>
       <c r="U40" s="40" t="s">
@@ -33135,19 +33140,19 @@
       <c r="E41" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="F41" s="144"/>
-      <c r="G41" s="145"/>
-      <c r="H41" s="146"/>
-      <c r="I41" s="147"/>
-      <c r="J41" s="148"/>
-      <c r="K41" s="148"/>
-      <c r="L41" s="149"/>
-      <c r="M41" s="153"/>
-      <c r="N41" s="154"/>
-      <c r="O41" s="154"/>
-      <c r="P41" s="154"/>
-      <c r="Q41" s="154"/>
-      <c r="R41" s="155"/>
+      <c r="F41" s="167"/>
+      <c r="G41" s="168"/>
+      <c r="H41" s="169"/>
+      <c r="I41" s="170"/>
+      <c r="J41" s="171"/>
+      <c r="K41" s="171"/>
+      <c r="L41" s="172"/>
+      <c r="M41" s="176"/>
+      <c r="N41" s="177"/>
+      <c r="O41" s="177"/>
+      <c r="P41" s="177"/>
+      <c r="Q41" s="177"/>
+      <c r="R41" s="178"/>
       <c r="S41" s="14"/>
       <c r="T41" s="14"/>
       <c r="U41" s="26" t="s">
@@ -33304,15 +33309,15 @@
       <c r="E46" s="53"/>
       <c r="F46" s="15"/>
       <c r="G46" s="15"/>
-      <c r="H46" s="123">
+      <c r="H46" s="146">
         <f>Extra!O2</f>
         <v>4</v>
       </c>
-      <c r="I46" s="124"/>
-      <c r="J46" s="124"/>
-      <c r="K46" s="124"/>
-      <c r="L46" s="124"/>
-      <c r="M46" s="125"/>
+      <c r="I46" s="147"/>
+      <c r="J46" s="147"/>
+      <c r="K46" s="147"/>
+      <c r="L46" s="147"/>
+      <c r="M46" s="148"/>
       <c r="N46" s="15"/>
       <c r="O46" s="15"/>
       <c r="P46" s="15"/>
@@ -33338,12 +33343,12 @@
       <c r="E47" s="57"/>
       <c r="F47" s="15"/>
       <c r="G47" s="15"/>
-      <c r="H47" s="126"/>
-      <c r="I47" s="127"/>
-      <c r="J47" s="127"/>
-      <c r="K47" s="127"/>
-      <c r="L47" s="127"/>
-      <c r="M47" s="128"/>
+      <c r="H47" s="149"/>
+      <c r="I47" s="150"/>
+      <c r="J47" s="150"/>
+      <c r="K47" s="150"/>
+      <c r="L47" s="150"/>
+      <c r="M47" s="151"/>
       <c r="N47" s="15"/>
       <c r="O47" s="15"/>
       <c r="P47" s="15"/>
@@ -33369,14 +33374,14 @@
       <c r="E48" s="63"/>
       <c r="F48" s="58"/>
       <c r="G48" s="58"/>
-      <c r="H48" s="129" t="s">
+      <c r="H48" s="152" t="s">
         <v>84</v>
       </c>
-      <c r="I48" s="130"/>
-      <c r="J48" s="130"/>
-      <c r="K48" s="130"/>
-      <c r="L48" s="130"/>
-      <c r="M48" s="130"/>
+      <c r="I48" s="153"/>
+      <c r="J48" s="153"/>
+      <c r="K48" s="153"/>
+      <c r="L48" s="153"/>
+      <c r="M48" s="153"/>
       <c r="N48" s="58"/>
       <c r="O48" s="58"/>
       <c r="P48" s="58"/>
@@ -33397,35 +33402,6 @@
     <protectedRange password="CA3F" sqref="E18 E34 Z9 E6 Z32 E25 Z17 Z24" name="Range1"/>
   </protectedRanges>
   <mergeCells count="40">
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="H4:K4"/>
-    <mergeCell ref="L4:O4"/>
-    <mergeCell ref="P4:S4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:S2"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="L3:O3"/>
-    <mergeCell ref="P3:S3"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F10"/>
-    <mergeCell ref="Z9:Z10"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="G12:M12"/>
-    <mergeCell ref="H13:J13"/>
-    <mergeCell ref="K13:M13"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="H14:J14"/>
-    <mergeCell ref="K14:M14"/>
-    <mergeCell ref="F16:F21"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="F23:F26"/>
-    <mergeCell ref="G23:R23"/>
-    <mergeCell ref="G24:R25"/>
-    <mergeCell ref="Z24:Z25"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="Z17:Z18"/>
     <mergeCell ref="H46:M47"/>
     <mergeCell ref="H48:M48"/>
     <mergeCell ref="Z28:Z29"/>
@@ -33437,6 +33413,35 @@
     <mergeCell ref="F40:H41"/>
     <mergeCell ref="I40:L41"/>
     <mergeCell ref="M40:R41"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="F23:F26"/>
+    <mergeCell ref="G23:R23"/>
+    <mergeCell ref="G24:R25"/>
+    <mergeCell ref="Z24:Z25"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="Z17:Z18"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="H14:J14"/>
+    <mergeCell ref="K14:M14"/>
+    <mergeCell ref="F16:F21"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F10"/>
+    <mergeCell ref="Z9:Z10"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="G12:M12"/>
+    <mergeCell ref="H13:J13"/>
+    <mergeCell ref="K13:M13"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:S2"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="L3:O3"/>
+    <mergeCell ref="P3:S3"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H4:K4"/>
+    <mergeCell ref="L4:O4"/>
+    <mergeCell ref="P4:S4"/>
   </mergeCells>
   <conditionalFormatting sqref="H46:M47">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="between">

</xml_diff>